<commit_message>
Cập nhật lại code 31.07.2018
</commit_message>
<xml_diff>
--- a/6. Schedule/SAMPLE_WBS.xlsx
+++ b/6. Schedule/SAMPLE_WBS.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="88">
   <si>
     <t>○</t>
     <phoneticPr fontId="5"/>
@@ -351,6 +351,21 @@
   </si>
   <si>
     <t>Viết chương trình quét SQL Injection trên DVWA</t>
+  </si>
+  <si>
+    <t>16.07.2018</t>
+  </si>
+  <si>
+    <t>22.07.2018</t>
+  </si>
+  <si>
+    <t>55ph</t>
+  </si>
+  <si>
+    <t>Quét thử trên website thật</t>
+  </si>
+  <si>
+    <t>60ph</t>
   </si>
 </sst>
 </file>
@@ -2003,6 +2018,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2021,16 +2042,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2055,18 +2066,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2082,6 +2081,28 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2102,12 +2123,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2168,6 +2183,9 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2176,9 +2194,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2190,7 +2205,7 @@
     <cellStyle name="Normal 2 2" xfId="6"/>
     <cellStyle name="Normal 3" xfId="5"/>
   </cellStyles>
-  <dxfs count="139">
+  <dxfs count="127">
     <dxf>
       <fill>
         <patternFill>
@@ -2587,90 +2602,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8585"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8585"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8585"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3666,10 +3597,10 @@
   <dimension ref="A1:EL120"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="18" ySplit="10" topLeftCell="Y36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="18" ySplit="10" topLeftCell="Y11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="W1" sqref="W1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="K37" sqref="K37:K38"/>
+      <selection pane="bottomRight" activeCell="AN44" sqref="AN44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -3797,18 +3728,18 @@
       <c r="K2" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="179" t="s">
+      <c r="L2" s="185" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="180"/>
-      <c r="N2" s="179" t="s">
+      <c r="M2" s="186"/>
+      <c r="N2" s="185" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="180"/>
+      <c r="O2" s="186"/>
       <c r="P2" s="118"/>
       <c r="Q2" s="207">
         <f ca="1">TODAY()</f>
-        <v>43296</v>
+        <v>43313</v>
       </c>
       <c r="R2" s="208"/>
       <c r="S2" s="35"/>
@@ -3942,7 +3873,7 @@
       <c r="EK2" s="40"/>
       <c r="EL2" s="15" t="str">
         <f ca="1">"Date："&amp;TEXT(TODAY()," yyyy/mm/dd")</f>
-        <v>Date： 2018/07/15</v>
+        <v>Date： 2018/08/01</v>
       </c>
     </row>
     <row r="3" spans="1:142" ht="18.75" customHeight="1">
@@ -3969,16 +3900,16 @@
         <f>COUNTIF(R11:R12,"=◇")</f>
         <v>0</v>
       </c>
-      <c r="L3" s="181">
+      <c r="L3" s="187">
         <f>COUNTIF(R11:R12,"=▲")</f>
         <v>0</v>
       </c>
-      <c r="M3" s="182"/>
-      <c r="N3" s="181">
+      <c r="M3" s="188"/>
+      <c r="N3" s="187">
         <f>COUNTIF(R11:R12,"=★")</f>
         <v>0</v>
       </c>
-      <c r="O3" s="182"/>
+      <c r="O3" s="188"/>
       <c r="P3" s="136"/>
       <c r="Q3" s="209"/>
       <c r="R3" s="209"/>
@@ -4636,47 +4567,47 @@
       </c>
     </row>
     <row r="9" spans="1:142" ht="14.25" customHeight="1">
-      <c r="B9" s="173" t="s">
+      <c r="B9" s="172" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="173" t="s">
+      <c r="C9" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="183" t="s">
+      <c r="D9" s="178" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="185" t="s">
+      <c r="E9" s="180" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="177" t="s">
+      <c r="F9" s="176" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="172" t="s">
+      <c r="G9" s="184" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="175" t="s">
+      <c r="H9" s="174" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="176"/>
-      <c r="J9" s="194" t="s">
+      <c r="I9" s="175"/>
+      <c r="J9" s="182" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="195"/>
-      <c r="L9" s="187" t="s">
+      <c r="K9" s="183"/>
+      <c r="L9" s="189" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="188"/>
-      <c r="N9" s="193" t="s">
+      <c r="M9" s="190"/>
+      <c r="N9" s="195" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="188"/>
-      <c r="P9" s="177" t="s">
+      <c r="O9" s="190"/>
+      <c r="P9" s="176" t="s">
         <v>43</v>
       </c>
-      <c r="Q9" s="189" t="s">
+      <c r="Q9" s="191" t="s">
         <v>39</v>
       </c>
-      <c r="R9" s="190"/>
+      <c r="R9" s="192"/>
       <c r="S9" s="29">
         <v>43282</v>
       </c>
@@ -5171,12 +5102,12 @@
       <c r="EL9" s="210"/>
     </row>
     <row r="10" spans="1:142" ht="14.25" customHeight="1">
-      <c r="B10" s="174"/>
-      <c r="C10" s="174"/>
-      <c r="D10" s="184"/>
-      <c r="E10" s="186"/>
-      <c r="F10" s="178"/>
-      <c r="G10" s="172"/>
+      <c r="B10" s="173"/>
+      <c r="C10" s="173"/>
+      <c r="D10" s="179"/>
+      <c r="E10" s="181"/>
+      <c r="F10" s="177"/>
+      <c r="G10" s="184"/>
       <c r="H10" s="112" t="s">
         <v>20</v>
       </c>
@@ -5201,9 +5132,9 @@
       <c r="O10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="P10" s="178"/>
-      <c r="Q10" s="191"/>
-      <c r="R10" s="192"/>
+      <c r="P10" s="177"/>
+      <c r="Q10" s="193"/>
+      <c r="R10" s="194"/>
       <c r="S10" s="22">
         <f>S9</f>
         <v>43282</v>
@@ -5544,13 +5475,13 @@
       <c r="D11" s="148"/>
       <c r="E11" s="146"/>
       <c r="F11" s="150"/>
-      <c r="G11" s="170" t="s">
+      <c r="G11" s="164" t="s">
         <v>62</v>
       </c>
       <c r="H11" s="156" t="s">
         <v>58</v>
       </c>
-      <c r="I11" s="164" t="s">
+      <c r="I11" s="166" t="s">
         <v>59</v>
       </c>
       <c r="J11" s="158" t="s">
@@ -5563,11 +5494,11 @@
       <c r="M11" s="154"/>
       <c r="N11" s="152"/>
       <c r="O11" s="154"/>
-      <c r="P11" s="168" t="s">
+      <c r="P11" s="170" t="s">
         <v>61</v>
       </c>
       <c r="Q11" s="160"/>
-      <c r="R11" s="166"/>
+      <c r="R11" s="168"/>
       <c r="S11" s="84"/>
       <c r="T11" s="87"/>
       <c r="U11" s="86"/>
@@ -5701,7 +5632,7 @@
       <c r="D12" s="149"/>
       <c r="E12" s="147"/>
       <c r="F12" s="151"/>
-      <c r="G12" s="171"/>
+      <c r="G12" s="165"/>
       <c r="H12" s="157"/>
       <c r="I12" s="157"/>
       <c r="J12" s="159"/>
@@ -5710,9 +5641,9 @@
       <c r="M12" s="155"/>
       <c r="N12" s="153"/>
       <c r="O12" s="155"/>
-      <c r="P12" s="169"/>
+      <c r="P12" s="171"/>
       <c r="Q12" s="161"/>
-      <c r="R12" s="167"/>
+      <c r="R12" s="169"/>
       <c r="S12" s="84"/>
       <c r="T12" s="85"/>
       <c r="U12" s="85"/>
@@ -5848,30 +5779,30 @@
       <c r="D13" s="148"/>
       <c r="E13" s="146"/>
       <c r="F13" s="150"/>
-      <c r="G13" s="170" t="s">
+      <c r="G13" s="164" t="s">
         <v>62</v>
       </c>
       <c r="H13" s="156" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="164" t="s">
+      <c r="I13" s="166" t="s">
         <v>59</v>
       </c>
       <c r="J13" s="158" t="s">
         <v>60</v>
       </c>
-      <c r="K13" s="164" t="s">
+      <c r="K13" s="166" t="s">
         <v>59</v>
       </c>
       <c r="L13" s="152"/>
       <c r="M13" s="154"/>
       <c r="N13" s="152"/>
       <c r="O13" s="154"/>
-      <c r="P13" s="168" t="s">
+      <c r="P13" s="170" t="s">
         <v>61</v>
       </c>
       <c r="Q13" s="160"/>
-      <c r="R13" s="166"/>
+      <c r="R13" s="168"/>
       <c r="S13" s="84"/>
       <c r="T13" s="87"/>
       <c r="U13" s="86"/>
@@ -6005,7 +5936,7 @@
       <c r="D14" s="149"/>
       <c r="E14" s="147"/>
       <c r="F14" s="151"/>
-      <c r="G14" s="171"/>
+      <c r="G14" s="165"/>
       <c r="H14" s="157"/>
       <c r="I14" s="157"/>
       <c r="J14" s="159"/>
@@ -6014,9 +5945,9 @@
       <c r="M14" s="155"/>
       <c r="N14" s="153"/>
       <c r="O14" s="155"/>
-      <c r="P14" s="169"/>
+      <c r="P14" s="171"/>
       <c r="Q14" s="161"/>
-      <c r="R14" s="167"/>
+      <c r="R14" s="169"/>
       <c r="S14" s="84"/>
       <c r="T14" s="85"/>
       <c r="U14" s="85"/>
@@ -6148,36 +6079,36 @@
       <c r="B15" s="162" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="165" t="s">
+      <c r="C15" s="167" t="s">
         <v>63</v>
       </c>
       <c r="D15" s="148"/>
       <c r="E15" s="146"/>
       <c r="F15" s="150"/>
-      <c r="G15" s="170" t="s">
+      <c r="G15" s="164" t="s">
         <v>62</v>
       </c>
       <c r="H15" s="156" t="s">
         <v>58</v>
       </c>
-      <c r="I15" s="164" t="s">
+      <c r="I15" s="166" t="s">
         <v>59</v>
       </c>
       <c r="J15" s="158" t="s">
         <v>60</v>
       </c>
-      <c r="K15" s="164" t="s">
+      <c r="K15" s="166" t="s">
         <v>59</v>
       </c>
       <c r="L15" s="152"/>
       <c r="M15" s="154"/>
       <c r="N15" s="152"/>
       <c r="O15" s="154"/>
-      <c r="P15" s="168" t="s">
+      <c r="P15" s="170" t="s">
         <v>61</v>
       </c>
       <c r="Q15" s="160"/>
-      <c r="R15" s="166"/>
+      <c r="R15" s="168"/>
       <c r="S15" s="84"/>
       <c r="T15" s="87"/>
       <c r="U15" s="86"/>
@@ -6307,11 +6238,11 @@
     </row>
     <row r="16" spans="1:142" ht="27" customHeight="1">
       <c r="B16" s="163"/>
-      <c r="C16" s="165"/>
+      <c r="C16" s="167"/>
       <c r="D16" s="149"/>
       <c r="E16" s="147"/>
       <c r="F16" s="151"/>
-      <c r="G16" s="171"/>
+      <c r="G16" s="165"/>
       <c r="H16" s="157"/>
       <c r="I16" s="157"/>
       <c r="J16" s="159"/>
@@ -6320,9 +6251,9 @@
       <c r="M16" s="155"/>
       <c r="N16" s="153"/>
       <c r="O16" s="155"/>
-      <c r="P16" s="169"/>
+      <c r="P16" s="171"/>
       <c r="Q16" s="161"/>
-      <c r="R16" s="167"/>
+      <c r="R16" s="169"/>
       <c r="S16" s="84"/>
       <c r="T16" s="85"/>
       <c r="U16" s="85"/>
@@ -6452,36 +6383,36 @@
     </row>
     <row r="17" spans="2:142" ht="27" customHeight="1">
       <c r="B17" s="162"/>
-      <c r="C17" s="165" t="s">
+      <c r="C17" s="167" t="s">
         <v>64</v>
       </c>
       <c r="D17" s="148"/>
       <c r="E17" s="146"/>
       <c r="F17" s="150"/>
-      <c r="G17" s="170" t="s">
+      <c r="G17" s="164" t="s">
         <v>62</v>
       </c>
       <c r="H17" s="156" t="s">
         <v>58</v>
       </c>
-      <c r="I17" s="164" t="s">
+      <c r="I17" s="166" t="s">
         <v>59</v>
       </c>
       <c r="J17" s="158" t="s">
         <v>60</v>
       </c>
-      <c r="K17" s="164" t="s">
+      <c r="K17" s="166" t="s">
         <v>59</v>
       </c>
       <c r="L17" s="152"/>
       <c r="M17" s="154"/>
       <c r="N17" s="152"/>
       <c r="O17" s="154"/>
-      <c r="P17" s="168" t="s">
+      <c r="P17" s="170" t="s">
         <v>61</v>
       </c>
       <c r="Q17" s="160"/>
-      <c r="R17" s="166"/>
+      <c r="R17" s="168"/>
       <c r="S17" s="84"/>
       <c r="T17" s="87"/>
       <c r="U17" s="86"/>
@@ -6611,11 +6542,11 @@
     </row>
     <row r="18" spans="2:142" ht="27" customHeight="1">
       <c r="B18" s="163"/>
-      <c r="C18" s="165"/>
+      <c r="C18" s="167"/>
       <c r="D18" s="149"/>
       <c r="E18" s="147"/>
       <c r="F18" s="151"/>
-      <c r="G18" s="171"/>
+      <c r="G18" s="165"/>
       <c r="H18" s="157"/>
       <c r="I18" s="157"/>
       <c r="J18" s="159"/>
@@ -6624,9 +6555,9 @@
       <c r="M18" s="155"/>
       <c r="N18" s="153"/>
       <c r="O18" s="155"/>
-      <c r="P18" s="169"/>
+      <c r="P18" s="171"/>
       <c r="Q18" s="161"/>
-      <c r="R18" s="167"/>
+      <c r="R18" s="169"/>
       <c r="S18" s="84"/>
       <c r="T18" s="85"/>
       <c r="U18" s="85"/>
@@ -6756,36 +6687,36 @@
     </row>
     <row r="19" spans="2:142" ht="27" customHeight="1">
       <c r="B19" s="162"/>
-      <c r="C19" s="165" t="s">
+      <c r="C19" s="167" t="s">
         <v>65</v>
       </c>
       <c r="D19" s="148"/>
       <c r="E19" s="146"/>
       <c r="F19" s="150"/>
-      <c r="G19" s="170" t="s">
+      <c r="G19" s="164" t="s">
         <v>62</v>
       </c>
       <c r="H19" s="156" t="s">
         <v>58</v>
       </c>
-      <c r="I19" s="164" t="s">
+      <c r="I19" s="166" t="s">
         <v>59</v>
       </c>
       <c r="J19" s="158" t="s">
         <v>60</v>
       </c>
-      <c r="K19" s="164" t="s">
+      <c r="K19" s="166" t="s">
         <v>59</v>
       </c>
       <c r="L19" s="152"/>
       <c r="M19" s="154"/>
       <c r="N19" s="152"/>
       <c r="O19" s="154"/>
-      <c r="P19" s="168" t="s">
+      <c r="P19" s="170" t="s">
         <v>61</v>
       </c>
       <c r="Q19" s="160"/>
-      <c r="R19" s="166"/>
+      <c r="R19" s="168"/>
       <c r="S19" s="84"/>
       <c r="T19" s="87"/>
       <c r="U19" s="86"/>
@@ -6915,11 +6846,11 @@
     </row>
     <row r="20" spans="2:142" ht="27" customHeight="1">
       <c r="B20" s="163"/>
-      <c r="C20" s="165"/>
+      <c r="C20" s="167"/>
       <c r="D20" s="149"/>
       <c r="E20" s="147"/>
       <c r="F20" s="151"/>
-      <c r="G20" s="171"/>
+      <c r="G20" s="165"/>
       <c r="H20" s="157"/>
       <c r="I20" s="157"/>
       <c r="J20" s="159"/>
@@ -6928,9 +6859,9 @@
       <c r="M20" s="155"/>
       <c r="N20" s="153"/>
       <c r="O20" s="155"/>
-      <c r="P20" s="169"/>
+      <c r="P20" s="171"/>
       <c r="Q20" s="161"/>
-      <c r="R20" s="167"/>
+      <c r="R20" s="169"/>
       <c r="S20" s="84"/>
       <c r="T20" s="85"/>
       <c r="U20" s="85"/>
@@ -7066,13 +6997,13 @@
       <c r="D21" s="148"/>
       <c r="E21" s="146"/>
       <c r="F21" s="150"/>
-      <c r="G21" s="170" t="s">
+      <c r="G21" s="164" t="s">
         <v>62</v>
       </c>
       <c r="H21" s="156" t="s">
         <v>59</v>
       </c>
-      <c r="I21" s="164" t="s">
+      <c r="I21" s="166" t="s">
         <v>76</v>
       </c>
       <c r="J21" s="158" t="s">
@@ -7085,11 +7016,11 @@
       <c r="M21" s="154"/>
       <c r="N21" s="152"/>
       <c r="O21" s="154"/>
-      <c r="P21" s="168" t="s">
+      <c r="P21" s="170" t="s">
         <v>61</v>
       </c>
       <c r="Q21" s="160"/>
-      <c r="R21" s="166"/>
+      <c r="R21" s="168"/>
       <c r="S21" s="84"/>
       <c r="T21" s="87"/>
       <c r="U21" s="86"/>
@@ -7223,7 +7154,7 @@
       <c r="D22" s="149"/>
       <c r="E22" s="147"/>
       <c r="F22" s="151"/>
-      <c r="G22" s="171"/>
+      <c r="G22" s="165"/>
       <c r="H22" s="157"/>
       <c r="I22" s="157"/>
       <c r="J22" s="159"/>
@@ -7232,9 +7163,9 @@
       <c r="M22" s="155"/>
       <c r="N22" s="153"/>
       <c r="O22" s="155"/>
-      <c r="P22" s="169"/>
+      <c r="P22" s="171"/>
       <c r="Q22" s="161"/>
-      <c r="R22" s="167"/>
+      <c r="R22" s="169"/>
       <c r="S22" s="84"/>
       <c r="T22" s="85"/>
       <c r="U22" s="85"/>
@@ -7370,13 +7301,13 @@
       <c r="D23" s="148"/>
       <c r="E23" s="146"/>
       <c r="F23" s="150"/>
-      <c r="G23" s="170" t="s">
+      <c r="G23" s="164" t="s">
         <v>62</v>
       </c>
       <c r="H23" s="156" t="s">
         <v>59</v>
       </c>
-      <c r="I23" s="164" t="s">
+      <c r="I23" s="166" t="s">
         <v>76</v>
       </c>
       <c r="J23" s="158" t="s">
@@ -7389,11 +7320,11 @@
       <c r="M23" s="154"/>
       <c r="N23" s="152"/>
       <c r="O23" s="154"/>
-      <c r="P23" s="168" t="s">
+      <c r="P23" s="170" t="s">
         <v>61</v>
       </c>
       <c r="Q23" s="160"/>
-      <c r="R23" s="166"/>
+      <c r="R23" s="168"/>
       <c r="S23" s="84"/>
       <c r="T23" s="87"/>
       <c r="U23" s="86"/>
@@ -7527,7 +7458,7 @@
       <c r="D24" s="149"/>
       <c r="E24" s="147"/>
       <c r="F24" s="151"/>
-      <c r="G24" s="171"/>
+      <c r="G24" s="165"/>
       <c r="H24" s="157"/>
       <c r="I24" s="157"/>
       <c r="J24" s="159"/>
@@ -7536,9 +7467,9 @@
       <c r="M24" s="155"/>
       <c r="N24" s="153"/>
       <c r="O24" s="155"/>
-      <c r="P24" s="169"/>
+      <c r="P24" s="171"/>
       <c r="Q24" s="161"/>
-      <c r="R24" s="167"/>
+      <c r="R24" s="169"/>
       <c r="S24" s="84"/>
       <c r="T24" s="85"/>
       <c r="U24" s="85"/>
@@ -7676,7 +7607,7 @@
       <c r="D25" s="148"/>
       <c r="E25" s="146"/>
       <c r="F25" s="150"/>
-      <c r="G25" s="170" t="s">
+      <c r="G25" s="164" t="s">
         <v>62</v>
       </c>
       <c r="H25" s="156" t="s">
@@ -7688,18 +7619,18 @@
       <c r="J25" s="158" t="s">
         <v>60</v>
       </c>
-      <c r="K25" s="164" t="s">
+      <c r="K25" s="166" t="s">
         <v>59</v>
       </c>
       <c r="L25" s="152"/>
       <c r="M25" s="154"/>
       <c r="N25" s="152"/>
       <c r="O25" s="154"/>
-      <c r="P25" s="168" t="s">
+      <c r="P25" s="170" t="s">
         <v>61</v>
       </c>
       <c r="Q25" s="160"/>
-      <c r="R25" s="166"/>
+      <c r="R25" s="168"/>
       <c r="S25" s="84"/>
       <c r="T25" s="87"/>
       <c r="U25" s="86"/>
@@ -7828,12 +7759,12 @@
       <c r="EL25" s="95"/>
     </row>
     <row r="26" spans="2:142" ht="27" customHeight="1">
-      <c r="B26" s="214"/>
+      <c r="B26" s="211"/>
       <c r="C26" s="145"/>
       <c r="D26" s="149"/>
       <c r="E26" s="147"/>
       <c r="F26" s="151"/>
-      <c r="G26" s="171"/>
+      <c r="G26" s="165"/>
       <c r="H26" s="157"/>
       <c r="I26" s="157"/>
       <c r="J26" s="159"/>
@@ -7842,9 +7773,9 @@
       <c r="M26" s="155"/>
       <c r="N26" s="153"/>
       <c r="O26" s="155"/>
-      <c r="P26" s="169"/>
+      <c r="P26" s="171"/>
       <c r="Q26" s="161"/>
-      <c r="R26" s="167"/>
+      <c r="R26" s="169"/>
       <c r="S26" s="84"/>
       <c r="T26" s="85"/>
       <c r="U26" s="85"/>
@@ -7973,37 +7904,37 @@
       <c r="EL26" s="96"/>
     </row>
     <row r="27" spans="2:142" ht="27" customHeight="1">
-      <c r="B27" s="214"/>
+      <c r="B27" s="211"/>
       <c r="C27" s="145" t="s">
         <v>51</v>
       </c>
       <c r="D27" s="148"/>
       <c r="E27" s="146"/>
       <c r="F27" s="150"/>
-      <c r="G27" s="170" t="s">
+      <c r="G27" s="164" t="s">
         <v>62</v>
       </c>
       <c r="H27" s="156" t="s">
         <v>58</v>
       </c>
-      <c r="I27" s="164" t="s">
+      <c r="I27" s="166" t="s">
         <v>59</v>
       </c>
       <c r="J27" s="158" t="s">
         <v>60</v>
       </c>
-      <c r="K27" s="164" t="s">
+      <c r="K27" s="166" t="s">
         <v>59</v>
       </c>
       <c r="L27" s="152"/>
       <c r="M27" s="154"/>
       <c r="N27" s="152"/>
       <c r="O27" s="154"/>
-      <c r="P27" s="168" t="s">
+      <c r="P27" s="170" t="s">
         <v>61</v>
       </c>
       <c r="Q27" s="160"/>
-      <c r="R27" s="166"/>
+      <c r="R27" s="168"/>
       <c r="S27" s="84"/>
       <c r="T27" s="87"/>
       <c r="U27" s="86"/>
@@ -8137,7 +8068,7 @@
       <c r="D28" s="149"/>
       <c r="E28" s="147"/>
       <c r="F28" s="151"/>
-      <c r="G28" s="171"/>
+      <c r="G28" s="165"/>
       <c r="H28" s="157"/>
       <c r="I28" s="157"/>
       <c r="J28" s="159"/>
@@ -8146,9 +8077,9 @@
       <c r="M28" s="155"/>
       <c r="N28" s="153"/>
       <c r="O28" s="155"/>
-      <c r="P28" s="169"/>
+      <c r="P28" s="171"/>
       <c r="Q28" s="161"/>
-      <c r="R28" s="167"/>
+      <c r="R28" s="169"/>
       <c r="S28" s="84"/>
       <c r="T28" s="85"/>
       <c r="U28" s="85"/>
@@ -8284,30 +8215,30 @@
       <c r="D29" s="148"/>
       <c r="E29" s="146"/>
       <c r="F29" s="150"/>
-      <c r="G29" s="170" t="s">
+      <c r="G29" s="164" t="s">
         <v>62</v>
       </c>
       <c r="H29" s="156" t="s">
         <v>58</v>
       </c>
-      <c r="I29" s="164" t="s">
+      <c r="I29" s="166" t="s">
         <v>59</v>
       </c>
       <c r="J29" s="158" t="s">
         <v>60</v>
       </c>
-      <c r="K29" s="164" t="s">
+      <c r="K29" s="166" t="s">
         <v>59</v>
       </c>
       <c r="L29" s="152"/>
       <c r="M29" s="154"/>
       <c r="N29" s="152"/>
       <c r="O29" s="154"/>
-      <c r="P29" s="168" t="s">
+      <c r="P29" s="170" t="s">
         <v>61</v>
       </c>
       <c r="Q29" s="160"/>
-      <c r="R29" s="166"/>
+      <c r="R29" s="168"/>
       <c r="S29" s="84"/>
       <c r="T29" s="87"/>
       <c r="U29" s="86"/>
@@ -8441,7 +8372,7 @@
       <c r="D30" s="149"/>
       <c r="E30" s="147"/>
       <c r="F30" s="151"/>
-      <c r="G30" s="171"/>
+      <c r="G30" s="165"/>
       <c r="H30" s="157"/>
       <c r="I30" s="157"/>
       <c r="J30" s="159"/>
@@ -8450,9 +8381,9 @@
       <c r="M30" s="155"/>
       <c r="N30" s="153"/>
       <c r="O30" s="155"/>
-      <c r="P30" s="169"/>
+      <c r="P30" s="171"/>
       <c r="Q30" s="161"/>
-      <c r="R30" s="167"/>
+      <c r="R30" s="169"/>
       <c r="S30" s="84"/>
       <c r="T30" s="85"/>
       <c r="U30" s="85"/>
@@ -8590,13 +8521,13 @@
       <c r="D31" s="148"/>
       <c r="E31" s="146"/>
       <c r="F31" s="150"/>
-      <c r="G31" s="170" t="s">
+      <c r="G31" s="164" t="s">
         <v>62</v>
       </c>
       <c r="H31" s="156" t="s">
         <v>59</v>
       </c>
-      <c r="I31" s="164" t="s">
+      <c r="I31" s="166" t="s">
         <v>76</v>
       </c>
       <c r="J31" s="158" t="s">
@@ -8609,11 +8540,11 @@
       <c r="M31" s="154"/>
       <c r="N31" s="152"/>
       <c r="O31" s="154"/>
-      <c r="P31" s="168" t="s">
+      <c r="P31" s="170" t="s">
         <v>61</v>
       </c>
       <c r="Q31" s="160"/>
-      <c r="R31" s="166"/>
+      <c r="R31" s="168"/>
       <c r="S31" s="84"/>
       <c r="T31" s="87"/>
       <c r="U31" s="86"/>
@@ -8742,12 +8673,12 @@
       <c r="EL31" s="95"/>
     </row>
     <row r="32" spans="2:142" ht="27" customHeight="1">
-      <c r="B32" s="214"/>
+      <c r="B32" s="211"/>
       <c r="C32" s="145"/>
       <c r="D32" s="149"/>
       <c r="E32" s="147"/>
       <c r="F32" s="151"/>
-      <c r="G32" s="171"/>
+      <c r="G32" s="165"/>
       <c r="H32" s="157"/>
       <c r="I32" s="157"/>
       <c r="J32" s="159"/>
@@ -8756,9 +8687,9 @@
       <c r="M32" s="155"/>
       <c r="N32" s="153"/>
       <c r="O32" s="155"/>
-      <c r="P32" s="169"/>
+      <c r="P32" s="171"/>
       <c r="Q32" s="161"/>
-      <c r="R32" s="167"/>
+      <c r="R32" s="169"/>
       <c r="S32" s="84"/>
       <c r="T32" s="85"/>
       <c r="U32" s="85"/>
@@ -8887,27 +8818,37 @@
       <c r="EL32" s="96"/>
     </row>
     <row r="33" spans="2:142" ht="27" customHeight="1">
-      <c r="B33" s="214"/>
+      <c r="B33" s="211"/>
       <c r="C33" s="145" t="s">
         <v>74</v>
       </c>
       <c r="D33" s="148"/>
       <c r="E33" s="146"/>
       <c r="F33" s="150"/>
-      <c r="G33" s="170" t="s">
+      <c r="G33" s="164" t="s">
         <v>62</v>
       </c>
-      <c r="H33" s="156"/>
-      <c r="I33" s="156"/>
-      <c r="J33" s="158"/>
-      <c r="K33" s="158"/>
+      <c r="H33" s="156" t="s">
+        <v>83</v>
+      </c>
+      <c r="I33" s="156" t="s">
+        <v>84</v>
+      </c>
+      <c r="J33" s="156" t="s">
+        <v>83</v>
+      </c>
+      <c r="K33" s="156" t="s">
+        <v>84</v>
+      </c>
       <c r="L33" s="152"/>
       <c r="M33" s="154"/>
       <c r="N33" s="152"/>
       <c r="O33" s="154"/>
-      <c r="P33" s="150"/>
+      <c r="P33" s="170" t="s">
+        <v>61</v>
+      </c>
       <c r="Q33" s="160"/>
-      <c r="R33" s="166"/>
+      <c r="R33" s="168"/>
       <c r="S33" s="84"/>
       <c r="T33" s="87"/>
       <c r="U33" s="86"/>
@@ -8923,7 +8864,9 @@
       <c r="AE33" s="86"/>
       <c r="AF33" s="86"/>
       <c r="AG33" s="86"/>
-      <c r="AH33" s="110"/>
+      <c r="AH33" s="110" t="s">
+        <v>70</v>
+      </c>
       <c r="AI33" s="110"/>
       <c r="AJ33" s="106"/>
       <c r="AK33" s="106"/>
@@ -9034,23 +8977,23 @@
       <c r="EL33" s="95"/>
     </row>
     <row r="34" spans="2:142" ht="27" customHeight="1">
-      <c r="B34" s="214"/>
+      <c r="B34" s="211"/>
       <c r="C34" s="145"/>
       <c r="D34" s="149"/>
       <c r="E34" s="147"/>
       <c r="F34" s="151"/>
-      <c r="G34" s="171"/>
+      <c r="G34" s="165"/>
       <c r="H34" s="157"/>
       <c r="I34" s="157"/>
-      <c r="J34" s="159"/>
-      <c r="K34" s="159"/>
+      <c r="J34" s="157"/>
+      <c r="K34" s="157"/>
       <c r="L34" s="153"/>
       <c r="M34" s="155"/>
       <c r="N34" s="153"/>
       <c r="O34" s="155"/>
-      <c r="P34" s="151"/>
+      <c r="P34" s="171"/>
       <c r="Q34" s="161"/>
-      <c r="R34" s="167"/>
+      <c r="R34" s="169"/>
       <c r="S34" s="84"/>
       <c r="T34" s="85"/>
       <c r="U34" s="85"/>
@@ -9066,7 +9009,9 @@
       <c r="AE34" s="85"/>
       <c r="AF34" s="85"/>
       <c r="AG34" s="85"/>
-      <c r="AH34" s="111"/>
+      <c r="AH34" s="111" t="s">
+        <v>85</v>
+      </c>
       <c r="AI34" s="111"/>
       <c r="AJ34" s="105"/>
       <c r="AK34" s="105"/>
@@ -9177,27 +9122,37 @@
       <c r="EL34" s="96"/>
     </row>
     <row r="35" spans="2:142" ht="27.6" customHeight="1">
-      <c r="B35" s="214"/>
+      <c r="B35" s="211"/>
       <c r="C35" s="145" t="s">
         <v>75</v>
       </c>
       <c r="D35" s="148"/>
       <c r="E35" s="146"/>
       <c r="F35" s="150"/>
-      <c r="G35" s="170" t="s">
+      <c r="G35" s="164" t="s">
         <v>62</v>
       </c>
-      <c r="H35" s="156"/>
-      <c r="I35" s="156"/>
-      <c r="J35" s="158"/>
-      <c r="K35" s="158"/>
+      <c r="H35" s="156" t="s">
+        <v>83</v>
+      </c>
+      <c r="I35" s="156" t="s">
+        <v>84</v>
+      </c>
+      <c r="J35" s="156" t="s">
+        <v>83</v>
+      </c>
+      <c r="K35" s="156" t="s">
+        <v>84</v>
+      </c>
       <c r="L35" s="152"/>
       <c r="M35" s="154"/>
       <c r="N35" s="152"/>
       <c r="O35" s="154"/>
-      <c r="P35" s="150"/>
+      <c r="P35" s="170" t="s">
+        <v>61</v>
+      </c>
       <c r="Q35" s="160"/>
-      <c r="R35" s="166"/>
+      <c r="R35" s="168"/>
       <c r="S35" s="84"/>
       <c r="T35" s="87"/>
       <c r="U35" s="86"/>
@@ -9214,7 +9169,9 @@
       <c r="AF35" s="86"/>
       <c r="AG35" s="86"/>
       <c r="AH35" s="110"/>
-      <c r="AI35" s="110"/>
+      <c r="AI35" s="110" t="s">
+        <v>70</v>
+      </c>
       <c r="AJ35" s="106"/>
       <c r="AK35" s="106"/>
       <c r="AL35" s="106"/>
@@ -9329,18 +9286,18 @@
       <c r="D36" s="149"/>
       <c r="E36" s="147"/>
       <c r="F36" s="151"/>
-      <c r="G36" s="171"/>
+      <c r="G36" s="165"/>
       <c r="H36" s="157"/>
       <c r="I36" s="157"/>
-      <c r="J36" s="159"/>
-      <c r="K36" s="159"/>
+      <c r="J36" s="157"/>
+      <c r="K36" s="157"/>
       <c r="L36" s="153"/>
       <c r="M36" s="155"/>
       <c r="N36" s="153"/>
       <c r="O36" s="155"/>
-      <c r="P36" s="151"/>
+      <c r="P36" s="171"/>
       <c r="Q36" s="161"/>
-      <c r="R36" s="167"/>
+      <c r="R36" s="169"/>
       <c r="S36" s="84"/>
       <c r="T36" s="85"/>
       <c r="U36" s="85"/>
@@ -9357,7 +9314,9 @@
       <c r="AF36" s="85"/>
       <c r="AG36" s="85"/>
       <c r="AH36" s="111"/>
-      <c r="AI36" s="111"/>
+      <c r="AI36" s="111" t="s">
+        <v>70</v>
+      </c>
       <c r="AJ36" s="105"/>
       <c r="AK36" s="105"/>
       <c r="AL36" s="105"/>
@@ -9476,20 +9435,28 @@
       <c r="D37" s="148"/>
       <c r="E37" s="146"/>
       <c r="F37" s="150"/>
-      <c r="G37" s="170" t="s">
+      <c r="G37" s="164" t="s">
         <v>62</v>
       </c>
-      <c r="H37" s="156"/>
-      <c r="I37" s="156"/>
-      <c r="J37" s="158"/>
-      <c r="K37" s="158"/>
+      <c r="H37" s="156" t="s">
+        <v>83</v>
+      </c>
+      <c r="I37" s="156" t="s">
+        <v>84</v>
+      </c>
+      <c r="J37" s="156" t="s">
+        <v>83</v>
+      </c>
+      <c r="K37" s="156" t="s">
+        <v>84</v>
+      </c>
       <c r="L37" s="152"/>
       <c r="M37" s="154"/>
       <c r="N37" s="152"/>
       <c r="O37" s="154"/>
       <c r="P37" s="150"/>
       <c r="Q37" s="160"/>
-      <c r="R37" s="166"/>
+      <c r="R37" s="168"/>
       <c r="S37" s="84"/>
       <c r="T37" s="87"/>
       <c r="U37" s="86"/>
@@ -9616,23 +9583,23 @@
       <c r="EL37" s="95"/>
     </row>
     <row r="38" spans="2:142" ht="27" customHeight="1">
-      <c r="B38" s="214"/>
+      <c r="B38" s="211"/>
       <c r="C38" s="145"/>
       <c r="D38" s="149"/>
       <c r="E38" s="147"/>
       <c r="F38" s="151"/>
-      <c r="G38" s="171"/>
+      <c r="G38" s="165"/>
       <c r="H38" s="157"/>
       <c r="I38" s="157"/>
-      <c r="J38" s="159"/>
-      <c r="K38" s="159"/>
+      <c r="J38" s="157"/>
+      <c r="K38" s="157"/>
       <c r="L38" s="153"/>
       <c r="M38" s="155"/>
       <c r="N38" s="153"/>
       <c r="O38" s="155"/>
       <c r="P38" s="151"/>
       <c r="Q38" s="161"/>
-      <c r="R38" s="167"/>
+      <c r="R38" s="169"/>
       <c r="S38" s="84"/>
       <c r="T38" s="85"/>
       <c r="U38" s="85"/>
@@ -9759,27 +9726,35 @@
       <c r="EL38" s="96"/>
     </row>
     <row r="39" spans="2:142" ht="27" customHeight="1">
-      <c r="B39" s="214"/>
+      <c r="B39" s="211"/>
       <c r="C39" s="145" t="s">
         <v>74</v>
       </c>
       <c r="D39" s="148"/>
       <c r="E39" s="146"/>
       <c r="F39" s="150"/>
-      <c r="G39" s="170" t="s">
+      <c r="G39" s="164" t="s">
         <v>62</v>
       </c>
-      <c r="H39" s="156"/>
-      <c r="I39" s="156"/>
-      <c r="J39" s="158"/>
-      <c r="K39" s="158"/>
+      <c r="H39" s="156" t="s">
+        <v>83</v>
+      </c>
+      <c r="I39" s="156" t="s">
+        <v>84</v>
+      </c>
+      <c r="J39" s="156" t="s">
+        <v>83</v>
+      </c>
+      <c r="K39" s="156" t="s">
+        <v>84</v>
+      </c>
       <c r="L39" s="152"/>
       <c r="M39" s="154"/>
       <c r="N39" s="152"/>
       <c r="O39" s="154"/>
       <c r="P39" s="150"/>
       <c r="Q39" s="160"/>
-      <c r="R39" s="166"/>
+      <c r="R39" s="168"/>
       <c r="S39" s="84"/>
       <c r="T39" s="87"/>
       <c r="U39" s="86"/>
@@ -9906,23 +9881,23 @@
       <c r="EL39" s="95"/>
     </row>
     <row r="40" spans="2:142" ht="27" customHeight="1">
-      <c r="B40" s="214"/>
+      <c r="B40" s="211"/>
       <c r="C40" s="145"/>
       <c r="D40" s="149"/>
       <c r="E40" s="147"/>
       <c r="F40" s="151"/>
-      <c r="G40" s="171"/>
+      <c r="G40" s="165"/>
       <c r="H40" s="157"/>
       <c r="I40" s="157"/>
-      <c r="J40" s="159"/>
-      <c r="K40" s="159"/>
+      <c r="J40" s="157"/>
+      <c r="K40" s="157"/>
       <c r="L40" s="153"/>
       <c r="M40" s="155"/>
       <c r="N40" s="153"/>
       <c r="O40" s="155"/>
       <c r="P40" s="151"/>
       <c r="Q40" s="161"/>
-      <c r="R40" s="167"/>
+      <c r="R40" s="169"/>
       <c r="S40" s="84"/>
       <c r="T40" s="85"/>
       <c r="U40" s="85"/>
@@ -10049,27 +10024,35 @@
       <c r="EL40" s="96"/>
     </row>
     <row r="41" spans="2:142" ht="27" customHeight="1">
-      <c r="B41" s="214"/>
+      <c r="B41" s="211"/>
       <c r="C41" s="145" t="s">
         <v>75</v>
       </c>
       <c r="D41" s="148"/>
       <c r="E41" s="146"/>
       <c r="F41" s="150"/>
-      <c r="G41" s="170" t="s">
+      <c r="G41" s="164" t="s">
         <v>62</v>
       </c>
-      <c r="H41" s="156"/>
-      <c r="I41" s="156"/>
-      <c r="J41" s="158"/>
-      <c r="K41" s="158"/>
+      <c r="H41" s="156" t="s">
+        <v>83</v>
+      </c>
+      <c r="I41" s="156" t="s">
+        <v>84</v>
+      </c>
+      <c r="J41" s="156" t="s">
+        <v>83</v>
+      </c>
+      <c r="K41" s="156" t="s">
+        <v>84</v>
+      </c>
       <c r="L41" s="152"/>
       <c r="M41" s="154"/>
       <c r="N41" s="152"/>
       <c r="O41" s="154"/>
       <c r="P41" s="150"/>
       <c r="Q41" s="160"/>
-      <c r="R41" s="166"/>
+      <c r="R41" s="168"/>
       <c r="S41" s="84"/>
       <c r="T41" s="87"/>
       <c r="U41" s="86"/>
@@ -10201,18 +10184,18 @@
       <c r="D42" s="149"/>
       <c r="E42" s="147"/>
       <c r="F42" s="151"/>
-      <c r="G42" s="171"/>
+      <c r="G42" s="165"/>
       <c r="H42" s="157"/>
       <c r="I42" s="157"/>
-      <c r="J42" s="159"/>
-      <c r="K42" s="159"/>
+      <c r="J42" s="157"/>
+      <c r="K42" s="157"/>
       <c r="L42" s="153"/>
       <c r="M42" s="155"/>
       <c r="N42" s="153"/>
       <c r="O42" s="155"/>
       <c r="P42" s="151"/>
       <c r="Q42" s="161"/>
-      <c r="R42" s="167"/>
+      <c r="R42" s="169"/>
       <c r="S42" s="84"/>
       <c r="T42" s="85"/>
       <c r="U42" s="85"/>
@@ -10338,24 +10321,38 @@
       <c r="EK42" s="104"/>
       <c r="EL42" s="96"/>
     </row>
-    <row r="43" spans="2:142" ht="9" customHeight="1">
-      <c r="B43" s="143"/>
+    <row r="43" spans="2:142" ht="27" customHeight="1">
+      <c r="B43" s="162" t="s">
+        <v>86</v>
+      </c>
       <c r="C43" s="145"/>
       <c r="D43" s="148"/>
       <c r="E43" s="146"/>
       <c r="F43" s="150"/>
-      <c r="G43" s="156"/>
-      <c r="H43" s="156"/>
-      <c r="I43" s="156"/>
-      <c r="J43" s="158"/>
-      <c r="K43" s="158"/>
+      <c r="G43" s="164" t="s">
+        <v>62</v>
+      </c>
+      <c r="H43" s="156" t="s">
+        <v>83</v>
+      </c>
+      <c r="I43" s="156" t="s">
+        <v>84</v>
+      </c>
+      <c r="J43" s="156" t="s">
+        <v>83</v>
+      </c>
+      <c r="K43" s="156" t="s">
+        <v>84</v>
+      </c>
       <c r="L43" s="152"/>
       <c r="M43" s="154"/>
       <c r="N43" s="152"/>
       <c r="O43" s="154"/>
-      <c r="P43" s="150"/>
+      <c r="P43" s="150" t="s">
+        <v>61</v>
+      </c>
       <c r="Q43" s="160"/>
-      <c r="R43" s="166"/>
+      <c r="R43" s="168"/>
       <c r="S43" s="84"/>
       <c r="T43" s="87"/>
       <c r="U43" s="86"/>
@@ -10377,7 +10374,9 @@
       <c r="AK43" s="106"/>
       <c r="AL43" s="106"/>
       <c r="AM43" s="86"/>
-      <c r="AN43" s="86"/>
+      <c r="AN43" s="86" t="s">
+        <v>87</v>
+      </c>
       <c r="AO43" s="86"/>
       <c r="AP43" s="86"/>
       <c r="AQ43" s="86"/>
@@ -10481,24 +10480,24 @@
       <c r="EK43" s="101"/>
       <c r="EL43" s="95"/>
     </row>
-    <row r="44" spans="2:142" ht="9" customHeight="1">
-      <c r="B44" s="144"/>
+    <row r="44" spans="2:142" ht="27" customHeight="1">
+      <c r="B44" s="163"/>
       <c r="C44" s="145"/>
       <c r="D44" s="149"/>
       <c r="E44" s="147"/>
       <c r="F44" s="151"/>
-      <c r="G44" s="157"/>
+      <c r="G44" s="165"/>
       <c r="H44" s="157"/>
       <c r="I44" s="157"/>
-      <c r="J44" s="159"/>
-      <c r="K44" s="159"/>
+      <c r="J44" s="157"/>
+      <c r="K44" s="157"/>
       <c r="L44" s="153"/>
       <c r="M44" s="155"/>
       <c r="N44" s="153"/>
       <c r="O44" s="155"/>
       <c r="P44" s="151"/>
       <c r="Q44" s="161"/>
-      <c r="R44" s="167"/>
+      <c r="R44" s="169"/>
       <c r="S44" s="84"/>
       <c r="T44" s="85"/>
       <c r="U44" s="85"/>
@@ -10520,7 +10519,9 @@
       <c r="AK44" s="105"/>
       <c r="AL44" s="105"/>
       <c r="AM44" s="85"/>
-      <c r="AN44" s="85"/>
+      <c r="AN44" s="85" t="s">
+        <v>87</v>
+      </c>
       <c r="AO44" s="85"/>
       <c r="AP44" s="85"/>
       <c r="AQ44" s="85"/>
@@ -10641,7 +10642,7 @@
       <c r="O45" s="154"/>
       <c r="P45" s="150"/>
       <c r="Q45" s="160"/>
-      <c r="R45" s="166"/>
+      <c r="R45" s="168"/>
       <c r="S45" s="84"/>
       <c r="T45" s="87"/>
       <c r="U45" s="86"/>
@@ -10784,7 +10785,7 @@
       <c r="O46" s="155"/>
       <c r="P46" s="151"/>
       <c r="Q46" s="161"/>
-      <c r="R46" s="167"/>
+      <c r="R46" s="169"/>
       <c r="S46" s="84"/>
       <c r="T46" s="85"/>
       <c r="U46" s="85"/>
@@ -10927,7 +10928,7 @@
       <c r="O47" s="154"/>
       <c r="P47" s="150"/>
       <c r="Q47" s="160"/>
-      <c r="R47" s="166"/>
+      <c r="R47" s="168"/>
       <c r="S47" s="84"/>
       <c r="T47" s="87"/>
       <c r="U47" s="86"/>
@@ -11070,7 +11071,7 @@
       <c r="O48" s="155"/>
       <c r="P48" s="151"/>
       <c r="Q48" s="161"/>
-      <c r="R48" s="167"/>
+      <c r="R48" s="169"/>
       <c r="S48" s="84"/>
       <c r="T48" s="85"/>
       <c r="U48" s="85"/>
@@ -11213,7 +11214,7 @@
       <c r="O49" s="154"/>
       <c r="P49" s="150"/>
       <c r="Q49" s="160"/>
-      <c r="R49" s="166"/>
+      <c r="R49" s="168"/>
       <c r="S49" s="84"/>
       <c r="T49" s="87"/>
       <c r="U49" s="86"/>
@@ -11356,7 +11357,7 @@
       <c r="O50" s="155"/>
       <c r="P50" s="151"/>
       <c r="Q50" s="161"/>
-      <c r="R50" s="167"/>
+      <c r="R50" s="169"/>
       <c r="S50" s="84"/>
       <c r="T50" s="85"/>
       <c r="U50" s="85"/>
@@ -11499,7 +11500,7 @@
       <c r="O51" s="154"/>
       <c r="P51" s="150"/>
       <c r="Q51" s="160"/>
-      <c r="R51" s="166"/>
+      <c r="R51" s="168"/>
       <c r="S51" s="84"/>
       <c r="T51" s="87"/>
       <c r="U51" s="86"/>
@@ -11642,7 +11643,7 @@
       <c r="O52" s="155"/>
       <c r="P52" s="151"/>
       <c r="Q52" s="161"/>
-      <c r="R52" s="167"/>
+      <c r="R52" s="169"/>
       <c r="S52" s="84"/>
       <c r="T52" s="85"/>
       <c r="U52" s="85"/>
@@ -11785,7 +11786,7 @@
       <c r="O53" s="154"/>
       <c r="P53" s="150"/>
       <c r="Q53" s="160"/>
-      <c r="R53" s="166"/>
+      <c r="R53" s="168"/>
       <c r="S53" s="84"/>
       <c r="T53" s="87"/>
       <c r="U53" s="86"/>
@@ -11928,7 +11929,7 @@
       <c r="O54" s="155"/>
       <c r="P54" s="151"/>
       <c r="Q54" s="161"/>
-      <c r="R54" s="167"/>
+      <c r="R54" s="169"/>
       <c r="S54" s="84"/>
       <c r="T54" s="85"/>
       <c r="U54" s="85"/>
@@ -12071,7 +12072,7 @@
       <c r="O55" s="154"/>
       <c r="P55" s="150"/>
       <c r="Q55" s="160"/>
-      <c r="R55" s="166"/>
+      <c r="R55" s="168"/>
       <c r="S55" s="84"/>
       <c r="T55" s="87"/>
       <c r="U55" s="86"/>
@@ -12214,7 +12215,7 @@
       <c r="O56" s="155"/>
       <c r="P56" s="151"/>
       <c r="Q56" s="161"/>
-      <c r="R56" s="167"/>
+      <c r="R56" s="169"/>
       <c r="S56" s="84"/>
       <c r="T56" s="85"/>
       <c r="U56" s="85"/>
@@ -12357,7 +12358,7 @@
       <c r="O57" s="154"/>
       <c r="P57" s="150"/>
       <c r="Q57" s="160"/>
-      <c r="R57" s="166"/>
+      <c r="R57" s="168"/>
       <c r="S57" s="84"/>
       <c r="T57" s="87"/>
       <c r="U57" s="86"/>
@@ -12500,7 +12501,7 @@
       <c r="O58" s="155"/>
       <c r="P58" s="151"/>
       <c r="Q58" s="161"/>
-      <c r="R58" s="167"/>
+      <c r="R58" s="169"/>
       <c r="S58" s="84"/>
       <c r="T58" s="85"/>
       <c r="U58" s="85"/>
@@ -12643,7 +12644,7 @@
       <c r="O59" s="154"/>
       <c r="P59" s="150"/>
       <c r="Q59" s="160"/>
-      <c r="R59" s="166"/>
+      <c r="R59" s="168"/>
       <c r="S59" s="84"/>
       <c r="T59" s="87"/>
       <c r="U59" s="86"/>
@@ -12786,7 +12787,7 @@
       <c r="O60" s="155"/>
       <c r="P60" s="151"/>
       <c r="Q60" s="161"/>
-      <c r="R60" s="167"/>
+      <c r="R60" s="169"/>
       <c r="S60" s="84"/>
       <c r="T60" s="85"/>
       <c r="U60" s="85"/>
@@ -12929,7 +12930,7 @@
       <c r="O61" s="154"/>
       <c r="P61" s="150"/>
       <c r="Q61" s="160"/>
-      <c r="R61" s="166"/>
+      <c r="R61" s="168"/>
       <c r="S61" s="84"/>
       <c r="T61" s="87"/>
       <c r="U61" s="86"/>
@@ -13072,7 +13073,7 @@
       <c r="O62" s="155"/>
       <c r="P62" s="151"/>
       <c r="Q62" s="161"/>
-      <c r="R62" s="167"/>
+      <c r="R62" s="169"/>
       <c r="S62" s="84"/>
       <c r="T62" s="85"/>
       <c r="U62" s="85"/>
@@ -13215,7 +13216,7 @@
       <c r="O63" s="154"/>
       <c r="P63" s="150"/>
       <c r="Q63" s="160"/>
-      <c r="R63" s="166"/>
+      <c r="R63" s="168"/>
       <c r="S63" s="84"/>
       <c r="T63" s="87"/>
       <c r="U63" s="86"/>
@@ -13358,7 +13359,7 @@
       <c r="O64" s="155"/>
       <c r="P64" s="151"/>
       <c r="Q64" s="161"/>
-      <c r="R64" s="167"/>
+      <c r="R64" s="169"/>
       <c r="S64" s="84"/>
       <c r="T64" s="85"/>
       <c r="U64" s="85"/>
@@ -13501,7 +13502,7 @@
       <c r="O65" s="154"/>
       <c r="P65" s="150"/>
       <c r="Q65" s="160"/>
-      <c r="R65" s="166"/>
+      <c r="R65" s="168"/>
       <c r="S65" s="84"/>
       <c r="T65" s="87"/>
       <c r="U65" s="86"/>
@@ -13644,7 +13645,7 @@
       <c r="O66" s="155"/>
       <c r="P66" s="151"/>
       <c r="Q66" s="161"/>
-      <c r="R66" s="167"/>
+      <c r="R66" s="169"/>
       <c r="S66" s="84"/>
       <c r="T66" s="85"/>
       <c r="U66" s="85"/>
@@ -13787,7 +13788,7 @@
       <c r="O67" s="154"/>
       <c r="P67" s="150"/>
       <c r="Q67" s="160"/>
-      <c r="R67" s="166"/>
+      <c r="R67" s="168"/>
       <c r="S67" s="84"/>
       <c r="T67" s="87"/>
       <c r="U67" s="86"/>
@@ -13930,7 +13931,7 @@
       <c r="O68" s="155"/>
       <c r="P68" s="151"/>
       <c r="Q68" s="161"/>
-      <c r="R68" s="167"/>
+      <c r="R68" s="169"/>
       <c r="S68" s="84"/>
       <c r="T68" s="85"/>
       <c r="U68" s="85"/>
@@ -14073,7 +14074,7 @@
       <c r="O69" s="154"/>
       <c r="P69" s="150"/>
       <c r="Q69" s="160"/>
-      <c r="R69" s="166"/>
+      <c r="R69" s="168"/>
       <c r="S69" s="84"/>
       <c r="T69" s="87"/>
       <c r="U69" s="86"/>
@@ -14216,7 +14217,7 @@
       <c r="O70" s="155"/>
       <c r="P70" s="151"/>
       <c r="Q70" s="161"/>
-      <c r="R70" s="167"/>
+      <c r="R70" s="169"/>
       <c r="S70" s="84"/>
       <c r="T70" s="85"/>
       <c r="U70" s="85"/>
@@ -14359,7 +14360,7 @@
       <c r="O71" s="154"/>
       <c r="P71" s="150"/>
       <c r="Q71" s="160"/>
-      <c r="R71" s="166"/>
+      <c r="R71" s="168"/>
       <c r="S71" s="84"/>
       <c r="T71" s="87"/>
       <c r="U71" s="86"/>
@@ -14502,7 +14503,7 @@
       <c r="O72" s="155"/>
       <c r="P72" s="151"/>
       <c r="Q72" s="161"/>
-      <c r="R72" s="167"/>
+      <c r="R72" s="169"/>
       <c r="S72" s="84"/>
       <c r="T72" s="85"/>
       <c r="U72" s="85"/>
@@ -14645,7 +14646,7 @@
       <c r="O73" s="154"/>
       <c r="P73" s="150"/>
       <c r="Q73" s="160"/>
-      <c r="R73" s="166"/>
+      <c r="R73" s="168"/>
       <c r="S73" s="84"/>
       <c r="T73" s="87"/>
       <c r="U73" s="86"/>
@@ -14788,7 +14789,7 @@
       <c r="O74" s="155"/>
       <c r="P74" s="151"/>
       <c r="Q74" s="161"/>
-      <c r="R74" s="167"/>
+      <c r="R74" s="169"/>
       <c r="S74" s="84"/>
       <c r="T74" s="85"/>
       <c r="U74" s="85"/>
@@ -14931,7 +14932,7 @@
       <c r="O75" s="154"/>
       <c r="P75" s="150"/>
       <c r="Q75" s="160"/>
-      <c r="R75" s="166"/>
+      <c r="R75" s="168"/>
       <c r="S75" s="84"/>
       <c r="T75" s="87"/>
       <c r="U75" s="86"/>
@@ -15074,7 +15075,7 @@
       <c r="O76" s="155"/>
       <c r="P76" s="151"/>
       <c r="Q76" s="161"/>
-      <c r="R76" s="167"/>
+      <c r="R76" s="169"/>
       <c r="S76" s="84"/>
       <c r="T76" s="85"/>
       <c r="U76" s="85"/>
@@ -15217,7 +15218,7 @@
       <c r="O77" s="154"/>
       <c r="P77" s="150"/>
       <c r="Q77" s="160"/>
-      <c r="R77" s="166"/>
+      <c r="R77" s="168"/>
       <c r="S77" s="84"/>
       <c r="T77" s="87"/>
       <c r="U77" s="86"/>
@@ -15360,7 +15361,7 @@
       <c r="O78" s="155"/>
       <c r="P78" s="151"/>
       <c r="Q78" s="161"/>
-      <c r="R78" s="167"/>
+      <c r="R78" s="169"/>
       <c r="S78" s="84"/>
       <c r="T78" s="85"/>
       <c r="U78" s="85"/>
@@ -15503,7 +15504,7 @@
       <c r="O79" s="154"/>
       <c r="P79" s="150"/>
       <c r="Q79" s="160"/>
-      <c r="R79" s="166"/>
+      <c r="R79" s="168"/>
       <c r="S79" s="84"/>
       <c r="T79" s="87"/>
       <c r="U79" s="86"/>
@@ -15646,7 +15647,7 @@
       <c r="O80" s="155"/>
       <c r="P80" s="151"/>
       <c r="Q80" s="161"/>
-      <c r="R80" s="167"/>
+      <c r="R80" s="169"/>
       <c r="S80" s="84"/>
       <c r="T80" s="85"/>
       <c r="U80" s="85"/>
@@ -15789,7 +15790,7 @@
       <c r="O81" s="154"/>
       <c r="P81" s="150"/>
       <c r="Q81" s="160"/>
-      <c r="R81" s="166"/>
+      <c r="R81" s="168"/>
       <c r="S81" s="84"/>
       <c r="T81" s="87"/>
       <c r="U81" s="86"/>
@@ -15932,7 +15933,7 @@
       <c r="O82" s="155"/>
       <c r="P82" s="151"/>
       <c r="Q82" s="161"/>
-      <c r="R82" s="167"/>
+      <c r="R82" s="169"/>
       <c r="S82" s="84"/>
       <c r="T82" s="85"/>
       <c r="U82" s="85"/>
@@ -16075,7 +16076,7 @@
       <c r="O83" s="154"/>
       <c r="P83" s="150"/>
       <c r="Q83" s="160"/>
-      <c r="R83" s="166"/>
+      <c r="R83" s="168"/>
       <c r="S83" s="84"/>
       <c r="T83" s="87"/>
       <c r="U83" s="86"/>
@@ -16218,7 +16219,7 @@
       <c r="O84" s="155"/>
       <c r="P84" s="151"/>
       <c r="Q84" s="161"/>
-      <c r="R84" s="167"/>
+      <c r="R84" s="169"/>
       <c r="S84" s="84"/>
       <c r="T84" s="85"/>
       <c r="U84" s="85"/>
@@ -16361,7 +16362,7 @@
       <c r="O85" s="154"/>
       <c r="P85" s="150"/>
       <c r="Q85" s="160"/>
-      <c r="R85" s="166"/>
+      <c r="R85" s="168"/>
       <c r="S85" s="84"/>
       <c r="T85" s="87"/>
       <c r="U85" s="86"/>
@@ -16504,7 +16505,7 @@
       <c r="O86" s="155"/>
       <c r="P86" s="151"/>
       <c r="Q86" s="161"/>
-      <c r="R86" s="167"/>
+      <c r="R86" s="169"/>
       <c r="S86" s="84"/>
       <c r="T86" s="85"/>
       <c r="U86" s="85"/>
@@ -16647,7 +16648,7 @@
       <c r="O87" s="154"/>
       <c r="P87" s="150"/>
       <c r="Q87" s="160"/>
-      <c r="R87" s="166"/>
+      <c r="R87" s="168"/>
       <c r="S87" s="84"/>
       <c r="T87" s="87"/>
       <c r="U87" s="86"/>
@@ -16790,7 +16791,7 @@
       <c r="O88" s="155"/>
       <c r="P88" s="151"/>
       <c r="Q88" s="161"/>
-      <c r="R88" s="167"/>
+      <c r="R88" s="169"/>
       <c r="S88" s="84"/>
       <c r="T88" s="85"/>
       <c r="U88" s="85"/>
@@ -16933,7 +16934,7 @@
       <c r="O89" s="154"/>
       <c r="P89" s="150"/>
       <c r="Q89" s="160"/>
-      <c r="R89" s="166"/>
+      <c r="R89" s="168"/>
       <c r="S89" s="84"/>
       <c r="T89" s="87"/>
       <c r="U89" s="86"/>
@@ -17076,7 +17077,7 @@
       <c r="O90" s="155"/>
       <c r="P90" s="151"/>
       <c r="Q90" s="161"/>
-      <c r="R90" s="167"/>
+      <c r="R90" s="169"/>
       <c r="S90" s="84"/>
       <c r="T90" s="85"/>
       <c r="U90" s="85"/>
@@ -17219,7 +17220,7 @@
       <c r="O91" s="154"/>
       <c r="P91" s="150"/>
       <c r="Q91" s="160"/>
-      <c r="R91" s="166"/>
+      <c r="R91" s="168"/>
       <c r="S91" s="84"/>
       <c r="T91" s="87"/>
       <c r="U91" s="86"/>
@@ -17362,7 +17363,7 @@
       <c r="O92" s="155"/>
       <c r="P92" s="151"/>
       <c r="Q92" s="161"/>
-      <c r="R92" s="167"/>
+      <c r="R92" s="169"/>
       <c r="S92" s="84"/>
       <c r="T92" s="85"/>
       <c r="U92" s="85"/>
@@ -17505,7 +17506,7 @@
       <c r="O93" s="154"/>
       <c r="P93" s="150"/>
       <c r="Q93" s="160"/>
-      <c r="R93" s="166"/>
+      <c r="R93" s="168"/>
       <c r="S93" s="84"/>
       <c r="T93" s="87"/>
       <c r="U93" s="86"/>
@@ -17648,7 +17649,7 @@
       <c r="O94" s="155"/>
       <c r="P94" s="151"/>
       <c r="Q94" s="161"/>
-      <c r="R94" s="167"/>
+      <c r="R94" s="169"/>
       <c r="S94" s="84"/>
       <c r="T94" s="85"/>
       <c r="U94" s="85"/>
@@ -17791,7 +17792,7 @@
       <c r="O95" s="154"/>
       <c r="P95" s="150"/>
       <c r="Q95" s="160"/>
-      <c r="R95" s="166"/>
+      <c r="R95" s="168"/>
       <c r="S95" s="84"/>
       <c r="T95" s="87"/>
       <c r="U95" s="86"/>
@@ -17934,7 +17935,7 @@
       <c r="O96" s="155"/>
       <c r="P96" s="151"/>
       <c r="Q96" s="161"/>
-      <c r="R96" s="167"/>
+      <c r="R96" s="169"/>
       <c r="S96" s="84"/>
       <c r="T96" s="85"/>
       <c r="U96" s="85"/>
@@ -18077,7 +18078,7 @@
       <c r="O97" s="154"/>
       <c r="P97" s="150"/>
       <c r="Q97" s="160"/>
-      <c r="R97" s="166"/>
+      <c r="R97" s="168"/>
       <c r="S97" s="84"/>
       <c r="T97" s="87"/>
       <c r="U97" s="86"/>
@@ -18220,7 +18221,7 @@
       <c r="O98" s="155"/>
       <c r="P98" s="151"/>
       <c r="Q98" s="161"/>
-      <c r="R98" s="167"/>
+      <c r="R98" s="169"/>
       <c r="S98" s="84"/>
       <c r="T98" s="85"/>
       <c r="U98" s="85"/>
@@ -18363,7 +18364,7 @@
       <c r="O99" s="154"/>
       <c r="P99" s="150"/>
       <c r="Q99" s="160"/>
-      <c r="R99" s="166"/>
+      <c r="R99" s="168"/>
       <c r="S99" s="84"/>
       <c r="T99" s="87"/>
       <c r="U99" s="86"/>
@@ -18506,7 +18507,7 @@
       <c r="O100" s="155"/>
       <c r="P100" s="151"/>
       <c r="Q100" s="161"/>
-      <c r="R100" s="167"/>
+      <c r="R100" s="169"/>
       <c r="S100" s="84"/>
       <c r="T100" s="85"/>
       <c r="U100" s="85"/>
@@ -18649,7 +18650,7 @@
       <c r="O101" s="154"/>
       <c r="P101" s="150"/>
       <c r="Q101" s="160"/>
-      <c r="R101" s="166"/>
+      <c r="R101" s="168"/>
       <c r="S101" s="84"/>
       <c r="T101" s="87"/>
       <c r="U101" s="86"/>
@@ -18792,7 +18793,7 @@
       <c r="O102" s="155"/>
       <c r="P102" s="151"/>
       <c r="Q102" s="161"/>
-      <c r="R102" s="167"/>
+      <c r="R102" s="169"/>
       <c r="S102" s="84"/>
       <c r="T102" s="85"/>
       <c r="U102" s="85"/>
@@ -18935,7 +18936,7 @@
       <c r="O103" s="154"/>
       <c r="P103" s="150"/>
       <c r="Q103" s="160"/>
-      <c r="R103" s="166"/>
+      <c r="R103" s="168"/>
       <c r="S103" s="84"/>
       <c r="T103" s="87"/>
       <c r="U103" s="86"/>
@@ -19078,7 +19079,7 @@
       <c r="O104" s="155"/>
       <c r="P104" s="151"/>
       <c r="Q104" s="161"/>
-      <c r="R104" s="167"/>
+      <c r="R104" s="169"/>
       <c r="S104" s="84"/>
       <c r="T104" s="85"/>
       <c r="U104" s="85"/>
@@ -19221,7 +19222,7 @@
       <c r="O105" s="154"/>
       <c r="P105" s="150"/>
       <c r="Q105" s="160"/>
-      <c r="R105" s="166"/>
+      <c r="R105" s="168"/>
       <c r="S105" s="84"/>
       <c r="T105" s="87"/>
       <c r="U105" s="86"/>
@@ -19364,7 +19365,7 @@
       <c r="O106" s="155"/>
       <c r="P106" s="151"/>
       <c r="Q106" s="161"/>
-      <c r="R106" s="167"/>
+      <c r="R106" s="169"/>
       <c r="S106" s="84"/>
       <c r="T106" s="85"/>
       <c r="U106" s="85"/>
@@ -19507,7 +19508,7 @@
       <c r="O107" s="154"/>
       <c r="P107" s="150"/>
       <c r="Q107" s="160"/>
-      <c r="R107" s="166"/>
+      <c r="R107" s="168"/>
       <c r="S107" s="84"/>
       <c r="T107" s="87"/>
       <c r="U107" s="86"/>
@@ -19650,7 +19651,7 @@
       <c r="O108" s="155"/>
       <c r="P108" s="151"/>
       <c r="Q108" s="161"/>
-      <c r="R108" s="167"/>
+      <c r="R108" s="169"/>
       <c r="S108" s="84"/>
       <c r="T108" s="85"/>
       <c r="U108" s="85"/>
@@ -19793,7 +19794,7 @@
       <c r="O109" s="154"/>
       <c r="P109" s="150"/>
       <c r="Q109" s="160"/>
-      <c r="R109" s="166"/>
+      <c r="R109" s="168"/>
       <c r="S109" s="84"/>
       <c r="T109" s="87"/>
       <c r="U109" s="86"/>
@@ -19936,7 +19937,7 @@
       <c r="O110" s="155"/>
       <c r="P110" s="151"/>
       <c r="Q110" s="161"/>
-      <c r="R110" s="167"/>
+      <c r="R110" s="169"/>
       <c r="S110" s="84"/>
       <c r="T110" s="85"/>
       <c r="U110" s="85"/>
@@ -20079,7 +20080,7 @@
       <c r="O111" s="154"/>
       <c r="P111" s="150"/>
       <c r="Q111" s="160"/>
-      <c r="R111" s="166"/>
+      <c r="R111" s="168"/>
       <c r="S111" s="84"/>
       <c r="T111" s="87"/>
       <c r="U111" s="86"/>
@@ -20222,7 +20223,7 @@
       <c r="O112" s="155"/>
       <c r="P112" s="151"/>
       <c r="Q112" s="161"/>
-      <c r="R112" s="167"/>
+      <c r="R112" s="169"/>
       <c r="S112" s="84"/>
       <c r="T112" s="85"/>
       <c r="U112" s="85"/>
@@ -20365,7 +20366,7 @@
       <c r="O113" s="154"/>
       <c r="P113" s="150"/>
       <c r="Q113" s="160"/>
-      <c r="R113" s="166"/>
+      <c r="R113" s="168"/>
       <c r="S113" s="84"/>
       <c r="T113" s="87"/>
       <c r="U113" s="86"/>
@@ -20508,7 +20509,7 @@
       <c r="O114" s="155"/>
       <c r="P114" s="151"/>
       <c r="Q114" s="161"/>
-      <c r="R114" s="167"/>
+      <c r="R114" s="169"/>
       <c r="S114" s="84"/>
       <c r="T114" s="85"/>
       <c r="U114" s="85"/>
@@ -20651,7 +20652,7 @@
       <c r="O115" s="154"/>
       <c r="P115" s="150"/>
       <c r="Q115" s="160"/>
-      <c r="R115" s="166"/>
+      <c r="R115" s="168"/>
       <c r="S115" s="84"/>
       <c r="T115" s="87"/>
       <c r="U115" s="86"/>
@@ -20794,7 +20795,7 @@
       <c r="O116" s="155"/>
       <c r="P116" s="151"/>
       <c r="Q116" s="161"/>
-      <c r="R116" s="167"/>
+      <c r="R116" s="169"/>
       <c r="S116" s="84"/>
       <c r="T116" s="85"/>
       <c r="U116" s="85"/>
@@ -20937,7 +20938,7 @@
       <c r="O117" s="154"/>
       <c r="P117" s="150"/>
       <c r="Q117" s="160"/>
-      <c r="R117" s="166"/>
+      <c r="R117" s="168"/>
       <c r="S117" s="84"/>
       <c r="T117" s="87"/>
       <c r="U117" s="86"/>
@@ -21080,7 +21081,7 @@
       <c r="O118" s="155"/>
       <c r="P118" s="151"/>
       <c r="Q118" s="161"/>
-      <c r="R118" s="167"/>
+      <c r="R118" s="169"/>
       <c r="S118" s="84"/>
       <c r="T118" s="85"/>
       <c r="U118" s="85"/>
@@ -21223,7 +21224,7 @@
       <c r="O119" s="154"/>
       <c r="P119" s="150"/>
       <c r="Q119" s="160"/>
-      <c r="R119" s="166"/>
+      <c r="R119" s="168"/>
       <c r="S119" s="84"/>
       <c r="T119" s="87"/>
       <c r="U119" s="86"/>
@@ -21366,7 +21367,7 @@
       <c r="O120" s="155"/>
       <c r="P120" s="151"/>
       <c r="Q120" s="161"/>
-      <c r="R120" s="167"/>
+      <c r="R120" s="169"/>
       <c r="S120" s="84"/>
       <c r="T120" s="85"/>
       <c r="U120" s="85"/>
@@ -21523,19 +21524,6 @@
     <mergeCell ref="P55:P56"/>
     <mergeCell ref="P57:P58"/>
     <mergeCell ref="M61:M62"/>
-    <mergeCell ref="N61:N62"/>
-    <mergeCell ref="J65:J66"/>
-    <mergeCell ref="K65:K66"/>
-    <mergeCell ref="N63:N64"/>
-    <mergeCell ref="O63:O64"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="I53:I54"/>
-    <mergeCell ref="J53:J54"/>
-    <mergeCell ref="K53:K54"/>
-    <mergeCell ref="L53:L54"/>
-    <mergeCell ref="M53:M54"/>
-    <mergeCell ref="N53:N54"/>
     <mergeCell ref="D55:D56"/>
     <mergeCell ref="H55:H56"/>
     <mergeCell ref="I55:I56"/>
@@ -21545,8 +21533,8 @@
     <mergeCell ref="M55:M56"/>
     <mergeCell ref="N55:N56"/>
     <mergeCell ref="G53:G54"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="J59:J60"/>
+    <mergeCell ref="R59:R60"/>
+    <mergeCell ref="M57:M58"/>
     <mergeCell ref="K59:K60"/>
     <mergeCell ref="L59:L60"/>
     <mergeCell ref="D61:D62"/>
@@ -21556,12 +21544,9 @@
     <mergeCell ref="J61:J62"/>
     <mergeCell ref="K61:K62"/>
     <mergeCell ref="L61:L62"/>
-    <mergeCell ref="K57:K58"/>
-    <mergeCell ref="L57:L58"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="N61:N62"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="J59:J60"/>
     <mergeCell ref="R61:R62"/>
     <mergeCell ref="G97:G98"/>
     <mergeCell ref="H97:H98"/>
@@ -21578,10 +21563,27 @@
     <mergeCell ref="G73:G74"/>
     <mergeCell ref="H73:H74"/>
     <mergeCell ref="I73:I74"/>
-    <mergeCell ref="R59:R60"/>
-    <mergeCell ref="M57:M58"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="P41:P42"/>
+    <mergeCell ref="J65:J66"/>
+    <mergeCell ref="K65:K66"/>
+    <mergeCell ref="N63:N64"/>
+    <mergeCell ref="O63:O64"/>
+    <mergeCell ref="L49:L50"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="N49:N50"/>
+    <mergeCell ref="O49:O50"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="K57:K58"/>
+    <mergeCell ref="L57:L58"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="I53:I54"/>
+    <mergeCell ref="J53:J54"/>
+    <mergeCell ref="K53:K54"/>
+    <mergeCell ref="L53:L54"/>
+    <mergeCell ref="M53:M54"/>
+    <mergeCell ref="N53:N54"/>
     <mergeCell ref="D51:D52"/>
     <mergeCell ref="H51:H52"/>
     <mergeCell ref="I51:I52"/>
@@ -21597,13 +21599,8 @@
     <mergeCell ref="I49:I50"/>
     <mergeCell ref="J49:J50"/>
     <mergeCell ref="K49:K50"/>
-    <mergeCell ref="L49:L50"/>
-    <mergeCell ref="M49:M50"/>
-    <mergeCell ref="N49:N50"/>
-    <mergeCell ref="O49:O50"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="E51:E52"/>
     <mergeCell ref="G117:G118"/>
     <mergeCell ref="H117:H118"/>
     <mergeCell ref="I117:I118"/>
@@ -21651,6 +21648,7 @@
     <mergeCell ref="N45:N46"/>
     <mergeCell ref="O45:O46"/>
     <mergeCell ref="Q45:Q46"/>
+    <mergeCell ref="P41:P42"/>
     <mergeCell ref="G119:G120"/>
     <mergeCell ref="H119:H120"/>
     <mergeCell ref="I119:I120"/>
@@ -21868,6 +21866,7 @@
     <mergeCell ref="I79:I80"/>
     <mergeCell ref="J79:J80"/>
     <mergeCell ref="K79:K80"/>
+    <mergeCell ref="D77:D78"/>
     <mergeCell ref="R77:R78"/>
     <mergeCell ref="E77:E78"/>
     <mergeCell ref="G77:G78"/>
@@ -21880,6 +21879,7 @@
     <mergeCell ref="Q73:Q74"/>
     <mergeCell ref="R73:R74"/>
     <mergeCell ref="K77:K78"/>
+    <mergeCell ref="Q69:Q70"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="H13:H14"/>
@@ -21923,6 +21923,8 @@
     <mergeCell ref="O11:O12"/>
     <mergeCell ref="Q11:Q12"/>
     <mergeCell ref="P13:P14"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="L11:L12"/>
     <mergeCell ref="Q37:Q38"/>
     <mergeCell ref="R37:R38"/>
     <mergeCell ref="N37:N38"/>
@@ -21935,6 +21937,7 @@
     <mergeCell ref="H37:H38"/>
     <mergeCell ref="I37:I38"/>
     <mergeCell ref="J37:J38"/>
+    <mergeCell ref="L37:L38"/>
     <mergeCell ref="R63:R64"/>
     <mergeCell ref="M71:M72"/>
     <mergeCell ref="N71:N72"/>
@@ -22005,6 +22008,8 @@
     <mergeCell ref="O17:O18"/>
     <mergeCell ref="O19:O20"/>
     <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="N17:N18"/>
     <mergeCell ref="BZ2:CB2"/>
     <mergeCell ref="CC2:CE2"/>
     <mergeCell ref="CF2:CH2"/>
@@ -22053,8 +22058,6 @@
     <mergeCell ref="P49:P50"/>
     <mergeCell ref="P51:P52"/>
     <mergeCell ref="Q41:Q42"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="L11:L12"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
@@ -22086,7 +22089,6 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="G9:G10"/>
-    <mergeCell ref="K27:K28"/>
     <mergeCell ref="E45:E46"/>
     <mergeCell ref="O93:O94"/>
     <mergeCell ref="Q93:Q94"/>
@@ -22108,8 +22110,9 @@
     <mergeCell ref="O75:O76"/>
     <mergeCell ref="Q75:Q76"/>
     <mergeCell ref="L83:L84"/>
-    <mergeCell ref="N17:N18"/>
     <mergeCell ref="L79:L80"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="H63:H64"/>
     <mergeCell ref="D71:D72"/>
     <mergeCell ref="D73:D74"/>
     <mergeCell ref="F99:F100"/>
@@ -22133,6 +22136,7 @@
     <mergeCell ref="E33:E34"/>
     <mergeCell ref="E35:E36"/>
     <mergeCell ref="G33:G34"/>
+    <mergeCell ref="E63:E64"/>
     <mergeCell ref="P31:P32"/>
     <mergeCell ref="G29:G30"/>
     <mergeCell ref="H29:H30"/>
@@ -22157,8 +22161,6 @@
     <mergeCell ref="E41:E42"/>
     <mergeCell ref="E43:E44"/>
     <mergeCell ref="G41:G42"/>
-    <mergeCell ref="L37:L38"/>
-    <mergeCell ref="N31:N32"/>
     <mergeCell ref="O31:O32"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="H21:H22"/>
@@ -22204,6 +22206,7 @@
     <mergeCell ref="K93:K94"/>
     <mergeCell ref="G99:G100"/>
     <mergeCell ref="H99:H100"/>
+    <mergeCell ref="O25:O26"/>
     <mergeCell ref="R27:R28"/>
     <mergeCell ref="J29:J30"/>
     <mergeCell ref="K29:K30"/>
@@ -22214,10 +22217,15 @@
     <mergeCell ref="Q29:Q30"/>
     <mergeCell ref="R29:R30"/>
     <mergeCell ref="P29:P30"/>
-    <mergeCell ref="N95:N96"/>
-    <mergeCell ref="L95:L96"/>
-    <mergeCell ref="R25:R26"/>
-    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="H67:H68"/>
+    <mergeCell ref="F87:F88"/>
+    <mergeCell ref="H53:H54"/>
     <mergeCell ref="E27:E28"/>
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="G27:G28"/>
@@ -22227,17 +22235,9 @@
     <mergeCell ref="N27:N28"/>
     <mergeCell ref="F39:F40"/>
     <mergeCell ref="F41:F42"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="H67:H68"/>
-    <mergeCell ref="F87:F88"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="N31:N32"/>
+    <mergeCell ref="H101:H102"/>
+    <mergeCell ref="I101:I102"/>
     <mergeCell ref="R21:R22"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="E23:E24"/>
@@ -22256,6 +22256,12 @@
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="F21:F22"/>
+    <mergeCell ref="N95:N96"/>
+    <mergeCell ref="L95:L96"/>
+    <mergeCell ref="R25:R26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
     <mergeCell ref="R93:R94"/>
     <mergeCell ref="H93:H94"/>
     <mergeCell ref="R17:R18"/>
@@ -22278,8 +22284,8 @@
     <mergeCell ref="F105:F106"/>
     <mergeCell ref="F107:F108"/>
     <mergeCell ref="J99:J100"/>
-    <mergeCell ref="H101:H102"/>
-    <mergeCell ref="I101:I102"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="H45:H46"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="G31:G32"/>
     <mergeCell ref="L31:L32"/>
@@ -22302,12 +22308,6 @@
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="C33:C34"/>
     <mergeCell ref="I33:I34"/>
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="C37:C38"/>
@@ -22317,20 +22317,25 @@
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D43:D44"/>
     <mergeCell ref="H43:H44"/>
     <mergeCell ref="I43:I44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="H65:H66"/>
-    <mergeCell ref="I65:I66"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
     <mergeCell ref="B47:B48"/>
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="B49:B50"/>
@@ -22341,17 +22346,6 @@
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="C55:C56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="H63:H64"/>
     <mergeCell ref="I63:I64"/>
     <mergeCell ref="D59:D60"/>
     <mergeCell ref="E59:E60"/>
@@ -22367,6 +22361,15 @@
     <mergeCell ref="N67:N68"/>
     <mergeCell ref="O67:O68"/>
     <mergeCell ref="Q67:Q68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="P67:P68"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="G65:G66"/>
+    <mergeCell ref="H65:H66"/>
+    <mergeCell ref="I65:I66"/>
+    <mergeCell ref="E61:E62"/>
     <mergeCell ref="B69:B70"/>
     <mergeCell ref="C69:C70"/>
     <mergeCell ref="E69:E70"/>
@@ -22376,9 +22379,7 @@
     <mergeCell ref="J69:J70"/>
     <mergeCell ref="K69:K70"/>
     <mergeCell ref="L69:L70"/>
-    <mergeCell ref="Q69:Q70"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="P67:P68"/>
+    <mergeCell ref="D69:D70"/>
     <mergeCell ref="L93:L94"/>
     <mergeCell ref="M93:M94"/>
     <mergeCell ref="N93:N94"/>
@@ -22460,371 +22461,470 @@
   </mergeCells>
   <phoneticPr fontId="5"/>
   <conditionalFormatting sqref="S8:EK8">
-    <cfRule type="expression" dxfId="138" priority="1814" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="1865" stopIfTrue="1">
       <formula>IF(TEXT(S$9,"d")="1",TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="1815" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="1866" stopIfTrue="1">
       <formula>OR(IF(TEXT(S$9,"d")&lt;&gt;"1",TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9:EK10">
-    <cfRule type="expression" dxfId="136" priority="1822" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="1873" stopIfTrue="1">
       <formula>IF(S$9=TODAY(),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="1823" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="1874" stopIfTrue="1">
       <formula>IF(WEEKDAY(S$9)=7,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="1824" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="1875" stopIfTrue="1">
       <formula>IF(OR(WEEKDAY(S$9)=1,IF(ISNA(MATCH(S$9,Holiday,0)),FALSE,TRUE)),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S11:EK120">
-    <cfRule type="expression" dxfId="133" priority="3504" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="3555" stopIfTrue="1">
       <formula>IF(OR(WEEKDAY(S$9)=7,WEEKDAY(S$9)=1,IF(ISNA(MATCH(S$9,Holiday,0)),FALSE,TRUE)),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="3505" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="3556" stopIfTrue="1">
       <formula>IF(AND($D11&lt;&gt;"",S11&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="3506" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="3557" stopIfTrue="1">
       <formula>IF(AND($D11="",S11&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J11:K11 B11:F11 B13:F13 J21:K21 B15:F15 B17:F17 C19:F19 C21:F21 C23:F23 C25:F25 J33:K33 J35:K35 C27:F27 C29:F29 B31:F31 C33:F33 C35:F35 J37:K37 B37 J39:K39 J41:K41 J43:K43 J45:K45 J47:K47 B43:F43 B45:F45 B47:F47 J49:K49 B49:F49 J51:K51 J53:K53 J55:K55 J57:K57 J59:K59 B51:F51 B53:F53 B55:F55 B57:F57 B59:F59 J61:K61 B61:F61 J63:K63 J65:K65 J67:K67 J69:K69 J71:K71 B63:F63 B65:F65 B67:F67 B69:F69 B71:F71 J73:K73 B73:F73 J75:K75 J77:K77 J79:K79 J81:K81 J83:K83 B75:F75 B77:F77 B79:F79 B81:F81 B83:F83 J85:K85 B85:F85 J87:K87 J89:K89 J91:K91 J93:K93 J95:K95 B87:F87 B89:F89 B91:F91 B93:F93 B95:F95 J97:K97 B97:F97 J99:K99 J101:K101 J103:K103 J105:K105 J107:K107 B99:F99 B101:F101 B103:F103 B105:F105 B107:F107 J109:K109 B109:F109 J111:K111 J113:K113 J115:K115 J117:K117 J119:K119 B111:F111 B113:F113 B115:F115 B117:F117 B119:F119 L11:O30 Q11:R120 G43:I120 G27:H30 G11:I26 L33:O120 D41:F41 D39:F39 D37:F37 H33:I42">
-    <cfRule type="expression" dxfId="130" priority="4957" stopIfTrue="1">
+  <conditionalFormatting sqref="J11:K11 B11:F11 B13:F13 J21:K21 B15:F15 B17:F17 C19:F19 C21:F21 C23:F23 C25:F25 C27:F27 C29:F29 B31:F31 C33:F33 C35:F35 B37 J45:K45 J47:K47 B43:F43 B45:F45 B47:F47 J49:K49 B49:F49 J51:K51 J53:K53 J55:K55 J57:K57 J59:K59 B51:F51 B53:F53 B55:F55 B57:F57 B59:F59 J61:K61 B61:F61 J63:K63 J65:K65 J67:K67 J69:K69 J71:K71 B63:F63 B65:F65 B67:F67 B69:F69 B71:F71 J73:K73 B73:F73 J75:K75 J77:K77 J79:K79 J81:K81 J83:K83 B75:F75 B77:F77 B79:F79 B81:F81 B83:F83 J85:K85 B85:F85 J87:K87 J89:K89 J91:K91 J93:K93 J95:K95 B87:F87 B89:F89 B91:F91 B93:F93 B95:F95 J97:K97 B97:F97 J99:K99 J101:K101 J103:K103 J105:K105 J107:K107 B99:F99 B101:F101 B103:F103 B105:F105 B107:F107 J109:K109 B109:F109 J111:K111 J113:K113 J115:K115 J117:K117 J119:K119 B111:F111 B113:F113 B115:F115 B117:F117 B119:F119 L11:O30 Q11:R120 G45:I120 G27:H30 G11:I26 L33:O120 D41:F41 D39:F39 D37:F37 H33:I36">
+    <cfRule type="expression" dxfId="118" priority="5008" stopIfTrue="1">
       <formula>IF(AND($D11&lt;&gt;"",$J11&lt;&gt;"",$K11&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="4958" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="5009" stopIfTrue="1">
       <formula>IF(AND($D11&lt;&gt;"",$K11="",$I11&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="4959" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="5010" stopIfTrue="1">
       <formula>IF(OR(AND($D11&lt;&gt;"",$J11&lt;&gt;"",$Q11&lt;100),TODAY()&gt;=$H11),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ11:DM120">
-    <cfRule type="expression" dxfId="127" priority="6037" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="6088" stopIfTrue="1">
       <formula>IF(OR(WEEKDAY(CJ$9)=7,WEEKDAY(CJ$9)=1,IF(ISNA(MATCH(CJ$9,Holiday,0)),FALSE,TRUE)),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="6038" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="6089" stopIfTrue="1">
       <formula>IF(AND($D11="",$S11&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P11 P33 P35 P37 P39 P41 P43 P45 P47 P49 P51 P53 P55 P57 P59 P61 P63 P65 P67 P69 P71 P73 P75 P77 P79 P81 P83 P85 P87 P89 P91 P93 P95 P97 P99 P101 P103 P105 P107 P109 P111 P113 P115 P117 P119">
-    <cfRule type="expression" dxfId="125" priority="206" stopIfTrue="1">
+  <conditionalFormatting sqref="P11 P37 P39 P41 P43 P45 P47 P49 P51 P53 P55 P57 P59 P61 P63 P65 P67 P69 P71 P73 P75 P77 P79 P81 P83 P85 P87 P89 P91 P93 P95 P97 P99 P101 P103 P105 P107 P109 P111 P113 P115 P117 P119">
+    <cfRule type="expression" dxfId="113" priority="257" stopIfTrue="1">
       <formula>IF(AND($D11&lt;&gt;"",$J11&lt;&gt;"",$K11&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="207" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="258" stopIfTrue="1">
       <formula>IF(AND($D11&lt;&gt;"",$K11="",$I11&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="208" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="259" stopIfTrue="1">
       <formula>IF(OR(AND($D11&lt;&gt;"",$J11&lt;&gt;"",$Q11&lt;100),TODAY()&gt;=$H11),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:K14">
-    <cfRule type="expression" dxfId="122" priority="136" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="187" stopIfTrue="1">
       <formula>IF(AND($D13&lt;&gt;"",$J13&lt;&gt;"",$K13&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="137" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="188" stopIfTrue="1">
       <formula>IF(AND($D13&lt;&gt;"",$K13="",$I13&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="138" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="189" stopIfTrue="1">
       <formula>IF(OR(AND($D13&lt;&gt;"",$J13&lt;&gt;"",$Q13&lt;100),TODAY()&gt;=$H13),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="expression" dxfId="119" priority="133" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="184" stopIfTrue="1">
       <formula>IF(AND($D13&lt;&gt;"",$J13&lt;&gt;"",$K13&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="134" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="185" stopIfTrue="1">
       <formula>IF(AND($D13&lt;&gt;"",$K13="",$I13&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="135" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="186" stopIfTrue="1">
       <formula>IF(OR(AND($D13&lt;&gt;"",$J13&lt;&gt;"",$Q13&lt;100),TODAY()&gt;=$H13),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P13">
-    <cfRule type="expression" dxfId="116" priority="130" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="181" stopIfTrue="1">
       <formula>IF(AND($D13&lt;&gt;"",$J13&lt;&gt;"",$K13&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="131" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="182" stopIfTrue="1">
       <formula>IF(AND($D13&lt;&gt;"",$K13="",$I13&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="132" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="183" stopIfTrue="1">
       <formula>IF(OR(AND($D13&lt;&gt;"",$J13&lt;&gt;"",$Q13&lt;100),TODAY()&gt;=$H13),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="expression" dxfId="113" priority="121" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="172" stopIfTrue="1">
       <formula>IF(AND($D19&lt;&gt;"",$J19&lt;&gt;"",$K19&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="122" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="173" stopIfTrue="1">
       <formula>IF(AND($D19&lt;&gt;"",$K19="",$I19&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="123" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="174" stopIfTrue="1">
       <formula>IF(OR(AND($D19&lt;&gt;"",$J19&lt;&gt;"",$Q19&lt;100),TODAY()&gt;=$H19),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="110" priority="118" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="169" stopIfTrue="1">
       <formula>IF(AND($D25&lt;&gt;"",$J25&lt;&gt;"",$K25&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="119" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="170" stopIfTrue="1">
       <formula>IF(AND($D25&lt;&gt;"",$K25="",$I25&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="120" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="171" stopIfTrue="1">
       <formula>IF(OR(AND($D25&lt;&gt;"",$J25&lt;&gt;"",$Q25&lt;100),TODAY()&gt;=$H25),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="107" priority="115" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="166" stopIfTrue="1">
       <formula>IF(AND($D23&lt;&gt;"",$J23&lt;&gt;"",$K23&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="116" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="167" stopIfTrue="1">
       <formula>IF(AND($D23&lt;&gt;"",$K23="",$I23&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="117" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="168" stopIfTrue="1">
       <formula>IF(OR(AND($D23&lt;&gt;"",$J23&lt;&gt;"",$Q23&lt;100),TODAY()&gt;=$H23),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="expression" dxfId="104" priority="112" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="163" stopIfTrue="1">
       <formula>IF(AND($D21&lt;&gt;"",$J21&lt;&gt;"",$K21&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="113" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="164" stopIfTrue="1">
       <formula>IF(AND($D21&lt;&gt;"",$K21="",$I21&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="114" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="165" stopIfTrue="1">
       <formula>IF(OR(AND($D21&lt;&gt;"",$J21&lt;&gt;"",$Q21&lt;100),TODAY()&gt;=$H21),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="expression" dxfId="101" priority="109" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="160" stopIfTrue="1">
       <formula>IF(AND($D29&lt;&gt;"",$J29&lt;&gt;"",$K29&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="110" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="161" stopIfTrue="1">
       <formula>IF(AND($D29&lt;&gt;"",$K29="",$I29&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="111" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="162" stopIfTrue="1">
       <formula>IF(OR(AND($D29&lt;&gt;"",$J29&lt;&gt;"",$Q29&lt;100),TODAY()&gt;=$H29),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:K20">
-    <cfRule type="expression" dxfId="98" priority="100" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="151" stopIfTrue="1">
       <formula>IF(AND($D15&lt;&gt;"",$J15&lt;&gt;"",$K15&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="101" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="152" stopIfTrue="1">
       <formula>IF(AND($D15&lt;&gt;"",$K15="",$I15&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="102" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="153" stopIfTrue="1">
       <formula>IF(OR(AND($D15&lt;&gt;"",$J15&lt;&gt;"",$Q15&lt;100),TODAY()&gt;=$H15),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25:K26">
-    <cfRule type="expression" dxfId="95" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="148" stopIfTrue="1">
       <formula>IF(AND($D25&lt;&gt;"",$J25&lt;&gt;"",$K25&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="149" stopIfTrue="1">
       <formula>IF(AND($D25&lt;&gt;"",$K25="",$I25&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="99" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="150" stopIfTrue="1">
       <formula>IF(OR(AND($D25&lt;&gt;"",$J25&lt;&gt;"",$Q25&lt;100),TODAY()&gt;=$H25),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P19 P17 P15">
-    <cfRule type="expression" dxfId="92" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="127" stopIfTrue="1">
       <formula>IF(AND($D15&lt;&gt;"",$J15&lt;&gt;"",$K15&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="128" stopIfTrue="1">
       <formula>IF(AND($D15&lt;&gt;"",$K15="",$I15&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="129" stopIfTrue="1">
       <formula>IF(OR(AND($D15&lt;&gt;"",$J15&lt;&gt;"",$Q15&lt;100),TODAY()&gt;=$H15),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P25">
-    <cfRule type="expression" dxfId="89" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="124" stopIfTrue="1">
       <formula>IF(AND($D25&lt;&gt;"",$J25&lt;&gt;"",$K25&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="125" stopIfTrue="1">
       <formula>IF(AND($D25&lt;&gt;"",$K25="",$I25&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="126" stopIfTrue="1">
       <formula>IF(OR(AND($D25&lt;&gt;"",$J25&lt;&gt;"",$Q25&lt;100),TODAY()&gt;=$H25),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19 J17 J15">
-    <cfRule type="expression" dxfId="86" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="109" stopIfTrue="1">
       <formula>IF(AND($D15&lt;&gt;"",$J15&lt;&gt;"",$K15&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="110" stopIfTrue="1">
       <formula>IF(AND($D15&lt;&gt;"",$K15="",$I15&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="111" stopIfTrue="1">
       <formula>IF(OR(AND($D15&lt;&gt;"",$J15&lt;&gt;"",$Q15&lt;100),TODAY()&gt;=$H15),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29">
-    <cfRule type="expression" dxfId="83" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="106" stopIfTrue="1">
       <formula>IF(AND($D29&lt;&gt;"",$J29&lt;&gt;"",$K29&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="107" stopIfTrue="1">
       <formula>IF(AND($D29&lt;&gt;"",$K29="",$I29&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="108" stopIfTrue="1">
       <formula>IF(OR(AND($D29&lt;&gt;"",$J29&lt;&gt;"",$Q29&lt;100),TODAY()&gt;=$H29),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25 J27">
-    <cfRule type="expression" dxfId="80" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="100" stopIfTrue="1">
       <formula>IF(AND($D25&lt;&gt;"",$J25&lt;&gt;"",$K25&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="101" stopIfTrue="1">
       <formula>IF(AND($D25&lt;&gt;"",$K25="",$I25&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="102" stopIfTrue="1">
       <formula>IF(OR(AND($D25&lt;&gt;"",$J25&lt;&gt;"",$Q25&lt;100),TODAY()&gt;=$H25),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27:K28">
-    <cfRule type="expression" dxfId="77" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="97" stopIfTrue="1">
       <formula>IF(AND($D27&lt;&gt;"",$J27&lt;&gt;"",$K27&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="98" stopIfTrue="1">
       <formula>IF(AND($D27&lt;&gt;"",$K27="",$I27&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="99" stopIfTrue="1">
       <formula>IF(OR(AND($D27&lt;&gt;"",$J27&lt;&gt;"",$Q27&lt;100),TODAY()&gt;=$H27),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:I30 K29:K30">
-    <cfRule type="expression" dxfId="74" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="88" stopIfTrue="1">
       <formula>IF(AND($D27&lt;&gt;"",$J27&lt;&gt;"",$K27&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="89" stopIfTrue="1">
       <formula>IF(AND($D27&lt;&gt;"",$K27="",$I27&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="90" stopIfTrue="1">
       <formula>IF(OR(AND($D27&lt;&gt;"",$J27&lt;&gt;"",$Q27&lt;100),TODAY()&gt;=$H27),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P29 P27">
-    <cfRule type="expression" dxfId="71" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="82" stopIfTrue="1">
       <formula>IF(AND($D27&lt;&gt;"",$J27&lt;&gt;"",$K27&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="83" stopIfTrue="1">
       <formula>IF(AND($D27&lt;&gt;"",$K27="",$I27&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="84" stopIfTrue="1">
       <formula>IF(OR(AND($D27&lt;&gt;"",$J27&lt;&gt;"",$Q27&lt;100),TODAY()&gt;=$H27),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31:G36">
-    <cfRule type="expression" dxfId="65" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="79" stopIfTrue="1">
       <formula>IF(AND($D31&lt;&gt;"",$J31&lt;&gt;"",$K31&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="80" stopIfTrue="1">
       <formula>IF(AND($D31&lt;&gt;"",$K31="",$I31&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="81" stopIfTrue="1">
       <formula>IF(OR(AND($D31&lt;&gt;"",$J31&lt;&gt;"",$Q31&lt;100),TODAY()&gt;=$H31),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23">
-    <cfRule type="expression" dxfId="53" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="76" stopIfTrue="1">
       <formula>IF(AND($D23&lt;&gt;"",$J23&lt;&gt;"",$K23&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="77" stopIfTrue="1">
       <formula>IF(AND($D23&lt;&gt;"",$K23="",$I23&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="78" stopIfTrue="1">
       <formula>IF(OR(AND($D23&lt;&gt;"",$J23&lt;&gt;"",$Q23&lt;100),TODAY()&gt;=$H23),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="expression" dxfId="47" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="73" stopIfTrue="1">
       <formula>IF(AND($D23&lt;&gt;"",$J23&lt;&gt;"",$K23&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="74" stopIfTrue="1">
       <formula>IF(AND($D23&lt;&gt;"",$K23="",$I23&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="75" stopIfTrue="1">
       <formula>IF(OR(AND($D23&lt;&gt;"",$J23&lt;&gt;"",$Q23&lt;100),TODAY()&gt;=$H23),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P23 P21">
-    <cfRule type="expression" dxfId="41" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="70" stopIfTrue="1">
       <formula>IF(AND($D21&lt;&gt;"",$J21&lt;&gt;"",$K21&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="71" stopIfTrue="1">
       <formula>IF(AND($D21&lt;&gt;"",$K21="",$I21&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="72" stopIfTrue="1">
       <formula>IF(OR(AND($D21&lt;&gt;"",$J21&lt;&gt;"",$Q21&lt;100),TODAY()&gt;=$H21),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L31:O32 H31:I32">
-    <cfRule type="expression" dxfId="35" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="67" stopIfTrue="1">
       <formula>IF(AND($D31&lt;&gt;"",$J31&lt;&gt;"",$K31&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="68" stopIfTrue="1">
       <formula>IF(AND($D31&lt;&gt;"",$K31="",$I31&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="69" stopIfTrue="1">
       <formula>IF(OR(AND($D31&lt;&gt;"",$J31&lt;&gt;"",$Q31&lt;100),TODAY()&gt;=$H31),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31">
-    <cfRule type="expression" dxfId="29" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="64" stopIfTrue="1">
       <formula>IF(AND($D31&lt;&gt;"",$J31&lt;&gt;"",$K31&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="65" stopIfTrue="1">
       <formula>IF(AND($D31&lt;&gt;"",$K31="",$I31&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="66" stopIfTrue="1">
       <formula>IF(OR(AND($D31&lt;&gt;"",$J31&lt;&gt;"",$Q31&lt;100),TODAY()&gt;=$H31),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="expression" dxfId="23" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="61" stopIfTrue="1">
       <formula>IF(AND($D31&lt;&gt;"",$J31&lt;&gt;"",$K31&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="62" stopIfTrue="1">
       <formula>IF(AND($D31&lt;&gt;"",$K31="",$I31&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="63" stopIfTrue="1">
       <formula>IF(OR(AND($D31&lt;&gt;"",$J31&lt;&gt;"",$Q31&lt;100),TODAY()&gt;=$H31),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P31">
-    <cfRule type="expression" dxfId="17" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="58" stopIfTrue="1">
       <formula>IF(AND($D31&lt;&gt;"",$J31&lt;&gt;"",$K31&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="59" stopIfTrue="1">
       <formula>IF(AND($D31&lt;&gt;"",$K31="",$I31&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="60" stopIfTrue="1">
       <formula>IF(OR(AND($D31&lt;&gt;"",$J31&lt;&gt;"",$Q31&lt;100),TODAY()&gt;=$H31),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37 C39 C41">
-    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="55" stopIfTrue="1">
       <formula>IF(AND($D37&lt;&gt;"",$J37&lt;&gt;"",$K37&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="56" stopIfTrue="1">
       <formula>IF(AND($D37&lt;&gt;"",$K37="",$I37&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="57" stopIfTrue="1">
       <formula>IF(OR(AND($D37&lt;&gt;"",$J37&lt;&gt;"",$Q37&lt;100),TODAY()&gt;=$H37),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37:G42">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="52" stopIfTrue="1">
       <formula>IF(AND($D37&lt;&gt;"",$J37&lt;&gt;"",$K37&lt;&gt;""),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="53" stopIfTrue="1">
       <formula>IF(AND($D37&lt;&gt;"",$K37="",$I37&lt;TODAY()),TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="54" stopIfTrue="1">
       <formula>IF(OR(AND($D37&lt;&gt;"",$J37&lt;&gt;"",$Q37&lt;100),TODAY()&gt;=$H37),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P33">
+    <cfRule type="expression" dxfId="26" priority="43" stopIfTrue="1">
+      <formula>IF(AND($D33&lt;&gt;"",$J33&lt;&gt;"",$K33&lt;&gt;""),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="44" stopIfTrue="1">
+      <formula>IF(AND($D33&lt;&gt;"",$K33="",$I33&lt;TODAY()),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="45" stopIfTrue="1">
+      <formula>IF(OR(AND($D33&lt;&gt;"",$J33&lt;&gt;"",$Q33&lt;100),TODAY()&gt;=$H33),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P35">
+    <cfRule type="expression" dxfId="23" priority="40" stopIfTrue="1">
+      <formula>IF(AND($D35&lt;&gt;"",$J35&lt;&gt;"",$K35&lt;&gt;""),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="41" stopIfTrue="1">
+      <formula>IF(AND($D35&lt;&gt;"",$K35="",$I35&lt;TODAY()),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="42" stopIfTrue="1">
+      <formula>IF(OR(AND($D35&lt;&gt;"",$J35&lt;&gt;"",$Q35&lt;100),TODAY()&gt;=$H35),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J33:K34">
+    <cfRule type="expression" dxfId="20" priority="31" stopIfTrue="1">
+      <formula>IF(AND($D33&lt;&gt;"",$J33&lt;&gt;"",$K33&lt;&gt;""),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="32" stopIfTrue="1">
+      <formula>IF(AND($D33&lt;&gt;"",$K33="",$I33&lt;TODAY()),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="33" stopIfTrue="1">
+      <formula>IF(OR(AND($D33&lt;&gt;"",$J33&lt;&gt;"",$Q33&lt;100),TODAY()&gt;=$H33),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J35:K36">
+    <cfRule type="expression" dxfId="17" priority="28" stopIfTrue="1">
+      <formula>IF(AND($D35&lt;&gt;"",$J35&lt;&gt;"",$K35&lt;&gt;""),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="29" stopIfTrue="1">
+      <formula>IF(AND($D35&lt;&gt;"",$K35="",$I35&lt;TODAY()),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="30" stopIfTrue="1">
+      <formula>IF(OR(AND($D35&lt;&gt;"",$J35&lt;&gt;"",$Q35&lt;100),TODAY()&gt;=$H35),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G43:G44">
+    <cfRule type="expression" dxfId="14" priority="25" stopIfTrue="1">
+      <formula>IF(AND($D43&lt;&gt;"",$J43&lt;&gt;"",$K43&lt;&gt;""),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="26" stopIfTrue="1">
+      <formula>IF(AND($D43&lt;&gt;"",$K43="",$I43&lt;TODAY()),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="27" stopIfTrue="1">
+      <formula>IF(OR(AND($D43&lt;&gt;"",$J43&lt;&gt;"",$Q43&lt;100),TODAY()&gt;=$H43),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H37:I42">
+    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
+      <formula>IF(AND($D37&lt;&gt;"",$J37&lt;&gt;"",$K37&lt;&gt;""),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
+      <formula>IF(AND($D37&lt;&gt;"",$K37="",$I37&lt;TODAY()),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
+      <formula>IF(OR(AND($D37&lt;&gt;"",$J37&lt;&gt;"",$Q37&lt;100),TODAY()&gt;=$H37),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J37:K42">
+    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
+      <formula>IF(AND($D37&lt;&gt;"",$J37&lt;&gt;"",$K37&lt;&gt;""),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+      <formula>IF(AND($D37&lt;&gt;"",$K37="",$I37&lt;TODAY()),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
+      <formula>IF(OR(AND($D37&lt;&gt;"",$J37&lt;&gt;"",$Q37&lt;100),TODAY()&gt;=$H37),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43:I44">
+    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+      <formula>IF(AND($D43&lt;&gt;"",$J43&lt;&gt;"",$K43&lt;&gt;""),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+      <formula>IF(AND($D43&lt;&gt;"",$K43="",$I43&lt;TODAY()),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+      <formula>IF(OR(AND($D43&lt;&gt;"",$J43&lt;&gt;"",$Q43&lt;100),TODAY()&gt;=$H43),TRUE,FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J43:K44">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+      <formula>IF(AND($D43&lt;&gt;"",$J43&lt;&gt;"",$K43&lt;&gt;""),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>IF(AND($D43&lt;&gt;"",$K43="",$I43&lt;TODAY()),TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+      <formula>IF(OR(AND($D43&lt;&gt;"",$J43&lt;&gt;"",$Q43&lt;100),TODAY()&gt;=$H43),TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -22863,11 +22963,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:23" ht="16.5" customHeight="1">
-      <c r="B3" s="211" t="s">
+      <c r="B3" s="212" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="212"/>
-      <c r="D3" s="213"/>
+      <c r="C3" s="213"/>
+      <c r="D3" s="214"/>
     </row>
     <row r="4" spans="2:23" ht="16.5" customHeight="1">
       <c r="B4" s="71" t="s">

</xml_diff>